<commit_message>
5/22 working time update
</commit_message>
<xml_diff>
--- a/Femto Project schedule V1.0.xlsx
+++ b/Femto Project schedule V1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="20180207" sheetId="18" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'20180328'!$A$1:$ND$54</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'20180423'!$A$1:$HT$54</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -283,7 +283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="184">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1019,6 +1019,10 @@
   </si>
   <si>
     <t>Commant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GEN Main Sch CON 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1994,7 +1998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="264">
+  <cellXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2367,6 +2371,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2457,19 +2472,11 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9383,167 +9390,167 @@
     </row>
     <row r="6" spans="1:152" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="235">
+      <c r="B6" s="240">
         <v>1</v>
       </c>
-      <c r="C6" s="232"/>
-      <c r="D6" s="232"/>
-      <c r="E6" s="232"/>
-      <c r="F6" s="232"/>
-      <c r="G6" s="232"/>
-      <c r="H6" s="232"/>
-      <c r="I6" s="232"/>
-      <c r="J6" s="232"/>
-      <c r="K6" s="232"/>
-      <c r="L6" s="232"/>
-      <c r="M6" s="232"/>
-      <c r="N6" s="232"/>
-      <c r="O6" s="232"/>
-      <c r="P6" s="232"/>
-      <c r="Q6" s="232"/>
-      <c r="R6" s="232"/>
-      <c r="S6" s="232"/>
-      <c r="T6" s="232"/>
-      <c r="U6" s="232"/>
-      <c r="V6" s="232"/>
-      <c r="W6" s="232"/>
-      <c r="X6" s="232"/>
-      <c r="Y6" s="232"/>
-      <c r="Z6" s="232"/>
-      <c r="AA6" s="232"/>
-      <c r="AB6" s="232"/>
-      <c r="AC6" s="232"/>
-      <c r="AD6" s="232"/>
-      <c r="AE6" s="232"/>
-      <c r="AF6" s="232"/>
-      <c r="AG6" s="235">
+      <c r="C6" s="237"/>
+      <c r="D6" s="237"/>
+      <c r="E6" s="237"/>
+      <c r="F6" s="237"/>
+      <c r="G6" s="237"/>
+      <c r="H6" s="237"/>
+      <c r="I6" s="237"/>
+      <c r="J6" s="237"/>
+      <c r="K6" s="237"/>
+      <c r="L6" s="237"/>
+      <c r="M6" s="237"/>
+      <c r="N6" s="237"/>
+      <c r="O6" s="237"/>
+      <c r="P6" s="237"/>
+      <c r="Q6" s="237"/>
+      <c r="R6" s="237"/>
+      <c r="S6" s="237"/>
+      <c r="T6" s="237"/>
+      <c r="U6" s="237"/>
+      <c r="V6" s="237"/>
+      <c r="W6" s="237"/>
+      <c r="X6" s="237"/>
+      <c r="Y6" s="237"/>
+      <c r="Z6" s="237"/>
+      <c r="AA6" s="237"/>
+      <c r="AB6" s="237"/>
+      <c r="AC6" s="237"/>
+      <c r="AD6" s="237"/>
+      <c r="AE6" s="237"/>
+      <c r="AF6" s="237"/>
+      <c r="AG6" s="240">
         <v>2</v>
       </c>
-      <c r="AH6" s="232"/>
-      <c r="AI6" s="232"/>
-      <c r="AJ6" s="232"/>
-      <c r="AK6" s="232"/>
-      <c r="AL6" s="232"/>
-      <c r="AM6" s="232"/>
-      <c r="AN6" s="232"/>
-      <c r="AO6" s="232"/>
-      <c r="AP6" s="232"/>
-      <c r="AQ6" s="232"/>
-      <c r="AR6" s="232"/>
-      <c r="AS6" s="232"/>
-      <c r="AT6" s="232"/>
-      <c r="AU6" s="232"/>
-      <c r="AV6" s="232"/>
-      <c r="AW6" s="232"/>
-      <c r="AX6" s="232"/>
-      <c r="AY6" s="232"/>
-      <c r="AZ6" s="232"/>
-      <c r="BA6" s="232"/>
-      <c r="BB6" s="232"/>
-      <c r="BC6" s="232"/>
-      <c r="BD6" s="232"/>
-      <c r="BE6" s="232"/>
-      <c r="BF6" s="232"/>
-      <c r="BG6" s="232"/>
-      <c r="BH6" s="233"/>
-      <c r="BI6" s="232">
+      <c r="AH6" s="237"/>
+      <c r="AI6" s="237"/>
+      <c r="AJ6" s="237"/>
+      <c r="AK6" s="237"/>
+      <c r="AL6" s="237"/>
+      <c r="AM6" s="237"/>
+      <c r="AN6" s="237"/>
+      <c r="AO6" s="237"/>
+      <c r="AP6" s="237"/>
+      <c r="AQ6" s="237"/>
+      <c r="AR6" s="237"/>
+      <c r="AS6" s="237"/>
+      <c r="AT6" s="237"/>
+      <c r="AU6" s="237"/>
+      <c r="AV6" s="237"/>
+      <c r="AW6" s="237"/>
+      <c r="AX6" s="237"/>
+      <c r="AY6" s="237"/>
+      <c r="AZ6" s="237"/>
+      <c r="BA6" s="237"/>
+      <c r="BB6" s="237"/>
+      <c r="BC6" s="237"/>
+      <c r="BD6" s="237"/>
+      <c r="BE6" s="237"/>
+      <c r="BF6" s="237"/>
+      <c r="BG6" s="237"/>
+      <c r="BH6" s="238"/>
+      <c r="BI6" s="237">
         <v>3</v>
       </c>
-      <c r="BJ6" s="232"/>
-      <c r="BK6" s="232"/>
-      <c r="BL6" s="232"/>
-      <c r="BM6" s="232"/>
-      <c r="BN6" s="232"/>
-      <c r="BO6" s="232"/>
-      <c r="BP6" s="232"/>
-      <c r="BQ6" s="232"/>
-      <c r="BR6" s="232"/>
-      <c r="BS6" s="232"/>
-      <c r="BT6" s="232"/>
-      <c r="BU6" s="232"/>
-      <c r="BV6" s="232"/>
-      <c r="BW6" s="232"/>
-      <c r="BX6" s="232"/>
-      <c r="BY6" s="232"/>
-      <c r="BZ6" s="232"/>
-      <c r="CA6" s="232"/>
-      <c r="CB6" s="232"/>
-      <c r="CC6" s="232"/>
-      <c r="CD6" s="232"/>
-      <c r="CE6" s="232"/>
-      <c r="CF6" s="232"/>
-      <c r="CG6" s="232"/>
-      <c r="CH6" s="232"/>
-      <c r="CI6" s="232"/>
-      <c r="CJ6" s="232"/>
-      <c r="CK6" s="232"/>
-      <c r="CL6" s="232"/>
-      <c r="CM6" s="232"/>
-      <c r="CN6" s="236">
+      <c r="BJ6" s="237"/>
+      <c r="BK6" s="237"/>
+      <c r="BL6" s="237"/>
+      <c r="BM6" s="237"/>
+      <c r="BN6" s="237"/>
+      <c r="BO6" s="237"/>
+      <c r="BP6" s="237"/>
+      <c r="BQ6" s="237"/>
+      <c r="BR6" s="237"/>
+      <c r="BS6" s="237"/>
+      <c r="BT6" s="237"/>
+      <c r="BU6" s="237"/>
+      <c r="BV6" s="237"/>
+      <c r="BW6" s="237"/>
+      <c r="BX6" s="237"/>
+      <c r="BY6" s="237"/>
+      <c r="BZ6" s="237"/>
+      <c r="CA6" s="237"/>
+      <c r="CB6" s="237"/>
+      <c r="CC6" s="237"/>
+      <c r="CD6" s="237"/>
+      <c r="CE6" s="237"/>
+      <c r="CF6" s="237"/>
+      <c r="CG6" s="237"/>
+      <c r="CH6" s="237"/>
+      <c r="CI6" s="237"/>
+      <c r="CJ6" s="237"/>
+      <c r="CK6" s="237"/>
+      <c r="CL6" s="237"/>
+      <c r="CM6" s="237"/>
+      <c r="CN6" s="241">
         <v>4</v>
       </c>
-      <c r="CO6" s="237"/>
-      <c r="CP6" s="237"/>
-      <c r="CQ6" s="237"/>
-      <c r="CR6" s="237"/>
-      <c r="CS6" s="237"/>
-      <c r="CT6" s="237"/>
-      <c r="CU6" s="237"/>
-      <c r="CV6" s="237"/>
-      <c r="CW6" s="237"/>
-      <c r="CX6" s="237"/>
-      <c r="CY6" s="237"/>
-      <c r="CZ6" s="237"/>
-      <c r="DA6" s="237"/>
-      <c r="DB6" s="237"/>
-      <c r="DC6" s="237"/>
-      <c r="DD6" s="237"/>
-      <c r="DE6" s="237"/>
-      <c r="DF6" s="237"/>
-      <c r="DG6" s="237"/>
-      <c r="DH6" s="237"/>
-      <c r="DI6" s="237"/>
-      <c r="DJ6" s="237"/>
-      <c r="DK6" s="237"/>
-      <c r="DL6" s="237"/>
-      <c r="DM6" s="237"/>
-      <c r="DN6" s="237"/>
-      <c r="DO6" s="237"/>
-      <c r="DP6" s="237"/>
-      <c r="DQ6" s="238"/>
-      <c r="DR6" s="232">
+      <c r="CO6" s="242"/>
+      <c r="CP6" s="242"/>
+      <c r="CQ6" s="242"/>
+      <c r="CR6" s="242"/>
+      <c r="CS6" s="242"/>
+      <c r="CT6" s="242"/>
+      <c r="CU6" s="242"/>
+      <c r="CV6" s="242"/>
+      <c r="CW6" s="242"/>
+      <c r="CX6" s="242"/>
+      <c r="CY6" s="242"/>
+      <c r="CZ6" s="242"/>
+      <c r="DA6" s="242"/>
+      <c r="DB6" s="242"/>
+      <c r="DC6" s="242"/>
+      <c r="DD6" s="242"/>
+      <c r="DE6" s="242"/>
+      <c r="DF6" s="242"/>
+      <c r="DG6" s="242"/>
+      <c r="DH6" s="242"/>
+      <c r="DI6" s="242"/>
+      <c r="DJ6" s="242"/>
+      <c r="DK6" s="242"/>
+      <c r="DL6" s="242"/>
+      <c r="DM6" s="242"/>
+      <c r="DN6" s="242"/>
+      <c r="DO6" s="242"/>
+      <c r="DP6" s="242"/>
+      <c r="DQ6" s="243"/>
+      <c r="DR6" s="237">
         <v>5</v>
       </c>
-      <c r="DS6" s="232"/>
-      <c r="DT6" s="232"/>
-      <c r="DU6" s="232"/>
-      <c r="DV6" s="232"/>
-      <c r="DW6" s="232"/>
-      <c r="DX6" s="232"/>
-      <c r="DY6" s="232"/>
-      <c r="DZ6" s="232"/>
-      <c r="EA6" s="232"/>
-      <c r="EB6" s="232"/>
-      <c r="EC6" s="232"/>
-      <c r="ED6" s="232"/>
-      <c r="EE6" s="232"/>
-      <c r="EF6" s="232"/>
-      <c r="EG6" s="232"/>
-      <c r="EH6" s="232"/>
-      <c r="EI6" s="232"/>
-      <c r="EJ6" s="232"/>
-      <c r="EK6" s="232"/>
-      <c r="EL6" s="232"/>
-      <c r="EM6" s="232"/>
-      <c r="EN6" s="232"/>
-      <c r="EO6" s="232"/>
-      <c r="EP6" s="232"/>
-      <c r="EQ6" s="232"/>
-      <c r="ER6" s="232"/>
-      <c r="ES6" s="232"/>
-      <c r="ET6" s="232"/>
-      <c r="EU6" s="232"/>
-      <c r="EV6" s="233"/>
+      <c r="DS6" s="237"/>
+      <c r="DT6" s="237"/>
+      <c r="DU6" s="237"/>
+      <c r="DV6" s="237"/>
+      <c r="DW6" s="237"/>
+      <c r="DX6" s="237"/>
+      <c r="DY6" s="237"/>
+      <c r="DZ6" s="237"/>
+      <c r="EA6" s="237"/>
+      <c r="EB6" s="237"/>
+      <c r="EC6" s="237"/>
+      <c r="ED6" s="237"/>
+      <c r="EE6" s="237"/>
+      <c r="EF6" s="237"/>
+      <c r="EG6" s="237"/>
+      <c r="EH6" s="237"/>
+      <c r="EI6" s="237"/>
+      <c r="EJ6" s="237"/>
+      <c r="EK6" s="237"/>
+      <c r="EL6" s="237"/>
+      <c r="EM6" s="237"/>
+      <c r="EN6" s="237"/>
+      <c r="EO6" s="237"/>
+      <c r="EP6" s="237"/>
+      <c r="EQ6" s="237"/>
+      <c r="ER6" s="237"/>
+      <c r="ES6" s="237"/>
+      <c r="ET6" s="237"/>
+      <c r="EU6" s="237"/>
+      <c r="EV6" s="238"/>
     </row>
     <row r="7" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -10002,7 +10009,7 @@
       </c>
     </row>
     <row r="8" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A8" s="229" t="s">
+      <c r="A8" s="234" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -10166,7 +10173,7 @@
       <c r="EV8" s="99"/>
     </row>
     <row r="9" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A9" s="229"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -10326,7 +10333,7 @@
       <c r="EV9" s="33"/>
     </row>
     <row r="10" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A10" s="229"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -10486,7 +10493,7 @@
       <c r="EV10" s="33"/>
     </row>
     <row r="11" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A11" s="229"/>
+      <c r="A11" s="234"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -10644,7 +10651,7 @@
       <c r="EV11" s="33"/>
     </row>
     <row r="12" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A12" s="229"/>
+      <c r="A12" s="234"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -10802,7 +10809,7 @@
       <c r="EV12" s="33"/>
     </row>
     <row r="13" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A13" s="229"/>
+      <c r="A13" s="234"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -10958,7 +10965,7 @@
       <c r="EV13" s="33"/>
     </row>
     <row r="14" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="234"/>
+      <c r="A14" s="239"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -11112,7 +11119,7 @@
       <c r="EV14" s="100"/>
     </row>
     <row r="15" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A15" s="231" t="s">
+      <c r="A15" s="236" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -11274,7 +11281,7 @@
       <c r="EV15" s="102"/>
     </row>
     <row r="16" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A16" s="229"/>
+      <c r="A16" s="234"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -11432,7 +11439,7 @@
       <c r="EV16" s="17"/>
     </row>
     <row r="17" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A17" s="229"/>
+      <c r="A17" s="234"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -11592,7 +11599,7 @@
       <c r="EV17" s="17"/>
     </row>
     <row r="18" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A18" s="229"/>
+      <c r="A18" s="234"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -11748,7 +11755,7 @@
       <c r="EV18" s="17"/>
     </row>
     <row r="19" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="229"/>
+      <c r="A19" s="234"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -11904,7 +11911,7 @@
       <c r="EV19" s="98"/>
     </row>
     <row r="20" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="231" t="s">
+      <c r="A20" s="236" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -12066,7 +12073,7 @@
       <c r="EV20" s="102"/>
     </row>
     <row r="21" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="229"/>
+      <c r="A21" s="234"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -12224,7 +12231,7 @@
       <c r="EV21" s="17"/>
     </row>
     <row r="22" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="229"/>
+      <c r="A22" s="234"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -12382,7 +12389,7 @@
       <c r="EV22" s="17"/>
     </row>
     <row r="23" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="229"/>
+      <c r="A23" s="234"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -12540,7 +12547,7 @@
       <c r="EV23" s="17"/>
     </row>
     <row r="24" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="230"/>
+      <c r="A24" s="235"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -12694,7 +12701,7 @@
       <c r="EV24" s="98"/>
     </row>
     <row r="25" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="231" t="s">
+      <c r="A25" s="236" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="75"/>
@@ -12850,7 +12857,7 @@
       <c r="EV25" s="102"/>
     </row>
     <row r="26" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="229"/>
+      <c r="A26" s="234"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -13004,7 +13011,7 @@
       <c r="EV26" s="17"/>
     </row>
     <row r="27" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="229"/>
+      <c r="A27" s="234"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -13158,7 +13165,7 @@
       <c r="EV27" s="17"/>
     </row>
     <row r="28" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="229"/>
+      <c r="A28" s="234"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -13312,7 +13319,7 @@
       <c r="EV28" s="17"/>
     </row>
     <row r="29" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="229"/>
+      <c r="A29" s="234"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -13466,7 +13473,7 @@
       <c r="EV29" s="98"/>
     </row>
     <row r="30" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="228" t="s">
+      <c r="A30" s="233" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="75"/>
@@ -13632,7 +13639,7 @@
       <c r="EV30" s="102"/>
     </row>
     <row r="31" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="229"/>
+      <c r="A31" s="234"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -13790,7 +13797,7 @@
       <c r="EV31" s="17"/>
     </row>
     <row r="32" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="229"/>
+      <c r="A32" s="234"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -13948,7 +13955,7 @@
       <c r="EV32" s="17"/>
     </row>
     <row r="33" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="229"/>
+      <c r="A33" s="234"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -14104,7 +14111,7 @@
       <c r="EV33" s="17"/>
     </row>
     <row r="34" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="230"/>
+      <c r="A34" s="235"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -14260,7 +14267,7 @@
       <c r="EV34" s="98"/>
     </row>
     <row r="35" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="229" t="s">
+      <c r="A35" s="234" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="75"/>
@@ -14418,7 +14425,7 @@
       <c r="EV35" s="102"/>
     </row>
     <row r="36" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="229"/>
+      <c r="A36" s="234"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -14574,7 +14581,7 @@
       <c r="EV36" s="17"/>
     </row>
     <row r="37" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="229"/>
+      <c r="A37" s="234"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -14728,7 +14735,7 @@
       <c r="EV37" s="17"/>
     </row>
     <row r="38" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="229"/>
+      <c r="A38" s="234"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -14882,7 +14889,7 @@
       <c r="EV38" s="17"/>
     </row>
     <row r="39" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="229"/>
+      <c r="A39" s="234"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -15036,7 +15043,7 @@
       <c r="EV39" s="98"/>
     </row>
     <row r="40" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="228" t="s">
+      <c r="A40" s="233" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="75"/>
@@ -15198,7 +15205,7 @@
       <c r="EV40" s="102"/>
     </row>
     <row r="41" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="229"/>
+      <c r="A41" s="234"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -15354,7 +15361,7 @@
       <c r="EV41" s="17"/>
     </row>
     <row r="42" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="229"/>
+      <c r="A42" s="234"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -15512,7 +15519,7 @@
       <c r="EV42" s="17"/>
     </row>
     <row r="43" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="229"/>
+      <c r="A43" s="234"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -15668,7 +15675,7 @@
       <c r="EV43" s="17"/>
     </row>
     <row r="44" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="230"/>
+      <c r="A44" s="235"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -15824,7 +15831,7 @@
       <c r="EV44" s="98"/>
     </row>
     <row r="45" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="229" t="s">
+      <c r="A45" s="234" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="75"/>
@@ -15986,7 +15993,7 @@
       <c r="EV45" s="102"/>
     </row>
     <row r="46" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="229"/>
+      <c r="A46" s="234"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -16142,7 +16149,7 @@
       <c r="EV46" s="17"/>
     </row>
     <row r="47" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="229"/>
+      <c r="A47" s="234"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -16300,7 +16307,7 @@
       <c r="EV47" s="17"/>
     </row>
     <row r="48" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="229"/>
+      <c r="A48" s="234"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -16456,7 +16463,7 @@
       <c r="EV48" s="17"/>
     </row>
     <row r="49" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="230"/>
+      <c r="A49" s="235"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -16692,395 +16699,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="235">
+      <c r="B6" s="240">
         <v>1</v>
       </c>
-      <c r="C6" s="232"/>
-      <c r="D6" s="232"/>
-      <c r="E6" s="232"/>
-      <c r="F6" s="232"/>
-      <c r="G6" s="232"/>
-      <c r="H6" s="232"/>
-      <c r="I6" s="232"/>
-      <c r="J6" s="232"/>
-      <c r="K6" s="232"/>
-      <c r="L6" s="232"/>
-      <c r="M6" s="232"/>
-      <c r="N6" s="232"/>
-      <c r="O6" s="232"/>
-      <c r="P6" s="232"/>
-      <c r="Q6" s="232"/>
-      <c r="R6" s="232"/>
-      <c r="S6" s="232"/>
-      <c r="T6" s="232"/>
-      <c r="U6" s="232"/>
-      <c r="V6" s="232"/>
-      <c r="W6" s="232"/>
-      <c r="X6" s="232"/>
-      <c r="Y6" s="232"/>
-      <c r="Z6" s="232"/>
-      <c r="AA6" s="232"/>
-      <c r="AB6" s="232"/>
-      <c r="AC6" s="232"/>
-      <c r="AD6" s="232"/>
-      <c r="AE6" s="232"/>
-      <c r="AF6" s="232"/>
-      <c r="AG6" s="235">
+      <c r="C6" s="237"/>
+      <c r="D6" s="237"/>
+      <c r="E6" s="237"/>
+      <c r="F6" s="237"/>
+      <c r="G6" s="237"/>
+      <c r="H6" s="237"/>
+      <c r="I6" s="237"/>
+      <c r="J6" s="237"/>
+      <c r="K6" s="237"/>
+      <c r="L6" s="237"/>
+      <c r="M6" s="237"/>
+      <c r="N6" s="237"/>
+      <c r="O6" s="237"/>
+      <c r="P6" s="237"/>
+      <c r="Q6" s="237"/>
+      <c r="R6" s="237"/>
+      <c r="S6" s="237"/>
+      <c r="T6" s="237"/>
+      <c r="U6" s="237"/>
+      <c r="V6" s="237"/>
+      <c r="W6" s="237"/>
+      <c r="X6" s="237"/>
+      <c r="Y6" s="237"/>
+      <c r="Z6" s="237"/>
+      <c r="AA6" s="237"/>
+      <c r="AB6" s="237"/>
+      <c r="AC6" s="237"/>
+      <c r="AD6" s="237"/>
+      <c r="AE6" s="237"/>
+      <c r="AF6" s="237"/>
+      <c r="AG6" s="240">
         <v>2</v>
       </c>
-      <c r="AH6" s="232"/>
-      <c r="AI6" s="232"/>
-      <c r="AJ6" s="232"/>
-      <c r="AK6" s="232"/>
-      <c r="AL6" s="232"/>
-      <c r="AM6" s="232"/>
-      <c r="AN6" s="232"/>
-      <c r="AO6" s="232"/>
-      <c r="AP6" s="232"/>
-      <c r="AQ6" s="232"/>
-      <c r="AR6" s="232"/>
-      <c r="AS6" s="232"/>
-      <c r="AT6" s="232"/>
-      <c r="AU6" s="232"/>
-      <c r="AV6" s="232"/>
-      <c r="AW6" s="232"/>
-      <c r="AX6" s="232"/>
-      <c r="AY6" s="232"/>
-      <c r="AZ6" s="232"/>
-      <c r="BA6" s="232"/>
-      <c r="BB6" s="232"/>
-      <c r="BC6" s="232"/>
-      <c r="BD6" s="232"/>
-      <c r="BE6" s="232"/>
-      <c r="BF6" s="232"/>
-      <c r="BG6" s="232"/>
-      <c r="BH6" s="233"/>
-      <c r="BI6" s="232">
+      <c r="AH6" s="237"/>
+      <c r="AI6" s="237"/>
+      <c r="AJ6" s="237"/>
+      <c r="AK6" s="237"/>
+      <c r="AL6" s="237"/>
+      <c r="AM6" s="237"/>
+      <c r="AN6" s="237"/>
+      <c r="AO6" s="237"/>
+      <c r="AP6" s="237"/>
+      <c r="AQ6" s="237"/>
+      <c r="AR6" s="237"/>
+      <c r="AS6" s="237"/>
+      <c r="AT6" s="237"/>
+      <c r="AU6" s="237"/>
+      <c r="AV6" s="237"/>
+      <c r="AW6" s="237"/>
+      <c r="AX6" s="237"/>
+      <c r="AY6" s="237"/>
+      <c r="AZ6" s="237"/>
+      <c r="BA6" s="237"/>
+      <c r="BB6" s="237"/>
+      <c r="BC6" s="237"/>
+      <c r="BD6" s="237"/>
+      <c r="BE6" s="237"/>
+      <c r="BF6" s="237"/>
+      <c r="BG6" s="237"/>
+      <c r="BH6" s="238"/>
+      <c r="BI6" s="237">
         <v>3</v>
       </c>
-      <c r="BJ6" s="232"/>
-      <c r="BK6" s="232"/>
-      <c r="BL6" s="232"/>
-      <c r="BM6" s="232"/>
-      <c r="BN6" s="232"/>
-      <c r="BO6" s="232"/>
-      <c r="BP6" s="232"/>
-      <c r="BQ6" s="232"/>
-      <c r="BR6" s="232"/>
-      <c r="BS6" s="232"/>
-      <c r="BT6" s="232"/>
-      <c r="BU6" s="232"/>
-      <c r="BV6" s="232"/>
-      <c r="BW6" s="232"/>
-      <c r="BX6" s="232"/>
-      <c r="BY6" s="232"/>
-      <c r="BZ6" s="232"/>
-      <c r="CA6" s="232"/>
-      <c r="CB6" s="232"/>
-      <c r="CC6" s="232"/>
-      <c r="CD6" s="232"/>
-      <c r="CE6" s="232"/>
-      <c r="CF6" s="232"/>
-      <c r="CG6" s="232"/>
-      <c r="CH6" s="232"/>
-      <c r="CI6" s="232"/>
-      <c r="CJ6" s="232"/>
-      <c r="CK6" s="232"/>
-      <c r="CL6" s="232"/>
-      <c r="CM6" s="232"/>
-      <c r="CN6" s="236">
+      <c r="BJ6" s="237"/>
+      <c r="BK6" s="237"/>
+      <c r="BL6" s="237"/>
+      <c r="BM6" s="237"/>
+      <c r="BN6" s="237"/>
+      <c r="BO6" s="237"/>
+      <c r="BP6" s="237"/>
+      <c r="BQ6" s="237"/>
+      <c r="BR6" s="237"/>
+      <c r="BS6" s="237"/>
+      <c r="BT6" s="237"/>
+      <c r="BU6" s="237"/>
+      <c r="BV6" s="237"/>
+      <c r="BW6" s="237"/>
+      <c r="BX6" s="237"/>
+      <c r="BY6" s="237"/>
+      <c r="BZ6" s="237"/>
+      <c r="CA6" s="237"/>
+      <c r="CB6" s="237"/>
+      <c r="CC6" s="237"/>
+      <c r="CD6" s="237"/>
+      <c r="CE6" s="237"/>
+      <c r="CF6" s="237"/>
+      <c r="CG6" s="237"/>
+      <c r="CH6" s="237"/>
+      <c r="CI6" s="237"/>
+      <c r="CJ6" s="237"/>
+      <c r="CK6" s="237"/>
+      <c r="CL6" s="237"/>
+      <c r="CM6" s="237"/>
+      <c r="CN6" s="241">
         <v>4</v>
       </c>
-      <c r="CO6" s="237"/>
-      <c r="CP6" s="237"/>
-      <c r="CQ6" s="237"/>
-      <c r="CR6" s="237"/>
-      <c r="CS6" s="237"/>
-      <c r="CT6" s="237"/>
-      <c r="CU6" s="237"/>
-      <c r="CV6" s="237"/>
-      <c r="CW6" s="237"/>
-      <c r="CX6" s="237"/>
-      <c r="CY6" s="237"/>
-      <c r="CZ6" s="237"/>
-      <c r="DA6" s="237"/>
-      <c r="DB6" s="237"/>
-      <c r="DC6" s="237"/>
-      <c r="DD6" s="237"/>
-      <c r="DE6" s="237"/>
-      <c r="DF6" s="237"/>
-      <c r="DG6" s="237"/>
-      <c r="DH6" s="237"/>
-      <c r="DI6" s="237"/>
-      <c r="DJ6" s="237"/>
-      <c r="DK6" s="237"/>
-      <c r="DL6" s="237"/>
-      <c r="DM6" s="237"/>
-      <c r="DN6" s="237"/>
-      <c r="DO6" s="237"/>
-      <c r="DP6" s="237"/>
-      <c r="DQ6" s="238"/>
-      <c r="DR6" s="232">
+      <c r="CO6" s="242"/>
+      <c r="CP6" s="242"/>
+      <c r="CQ6" s="242"/>
+      <c r="CR6" s="242"/>
+      <c r="CS6" s="242"/>
+      <c r="CT6" s="242"/>
+      <c r="CU6" s="242"/>
+      <c r="CV6" s="242"/>
+      <c r="CW6" s="242"/>
+      <c r="CX6" s="242"/>
+      <c r="CY6" s="242"/>
+      <c r="CZ6" s="242"/>
+      <c r="DA6" s="242"/>
+      <c r="DB6" s="242"/>
+      <c r="DC6" s="242"/>
+      <c r="DD6" s="242"/>
+      <c r="DE6" s="242"/>
+      <c r="DF6" s="242"/>
+      <c r="DG6" s="242"/>
+      <c r="DH6" s="242"/>
+      <c r="DI6" s="242"/>
+      <c r="DJ6" s="242"/>
+      <c r="DK6" s="242"/>
+      <c r="DL6" s="242"/>
+      <c r="DM6" s="242"/>
+      <c r="DN6" s="242"/>
+      <c r="DO6" s="242"/>
+      <c r="DP6" s="242"/>
+      <c r="DQ6" s="243"/>
+      <c r="DR6" s="237">
         <v>5</v>
       </c>
-      <c r="DS6" s="232"/>
-      <c r="DT6" s="232"/>
-      <c r="DU6" s="232"/>
-      <c r="DV6" s="232"/>
-      <c r="DW6" s="232"/>
-      <c r="DX6" s="232"/>
-      <c r="DY6" s="232"/>
-      <c r="DZ6" s="232"/>
-      <c r="EA6" s="232"/>
-      <c r="EB6" s="232"/>
-      <c r="EC6" s="232"/>
-      <c r="ED6" s="232"/>
-      <c r="EE6" s="232"/>
-      <c r="EF6" s="232"/>
-      <c r="EG6" s="232"/>
-      <c r="EH6" s="232"/>
-      <c r="EI6" s="232"/>
-      <c r="EJ6" s="232"/>
-      <c r="EK6" s="232"/>
-      <c r="EL6" s="232"/>
-      <c r="EM6" s="232"/>
-      <c r="EN6" s="232"/>
-      <c r="EO6" s="232"/>
-      <c r="EP6" s="232"/>
-      <c r="EQ6" s="232"/>
-      <c r="ER6" s="232"/>
-      <c r="ES6" s="232"/>
-      <c r="ET6" s="232"/>
-      <c r="EU6" s="232"/>
-      <c r="EV6" s="233"/>
-      <c r="EW6" s="236">
+      <c r="DS6" s="237"/>
+      <c r="DT6" s="237"/>
+      <c r="DU6" s="237"/>
+      <c r="DV6" s="237"/>
+      <c r="DW6" s="237"/>
+      <c r="DX6" s="237"/>
+      <c r="DY6" s="237"/>
+      <c r="DZ6" s="237"/>
+      <c r="EA6" s="237"/>
+      <c r="EB6" s="237"/>
+      <c r="EC6" s="237"/>
+      <c r="ED6" s="237"/>
+      <c r="EE6" s="237"/>
+      <c r="EF6" s="237"/>
+      <c r="EG6" s="237"/>
+      <c r="EH6" s="237"/>
+      <c r="EI6" s="237"/>
+      <c r="EJ6" s="237"/>
+      <c r="EK6" s="237"/>
+      <c r="EL6" s="237"/>
+      <c r="EM6" s="237"/>
+      <c r="EN6" s="237"/>
+      <c r="EO6" s="237"/>
+      <c r="EP6" s="237"/>
+      <c r="EQ6" s="237"/>
+      <c r="ER6" s="237"/>
+      <c r="ES6" s="237"/>
+      <c r="ET6" s="237"/>
+      <c r="EU6" s="237"/>
+      <c r="EV6" s="238"/>
+      <c r="EW6" s="241">
         <v>6</v>
       </c>
-      <c r="EX6" s="237"/>
-      <c r="EY6" s="237"/>
-      <c r="EZ6" s="237"/>
-      <c r="FA6" s="237"/>
-      <c r="FB6" s="237"/>
-      <c r="FC6" s="237"/>
-      <c r="FD6" s="237"/>
-      <c r="FE6" s="237"/>
-      <c r="FF6" s="237"/>
-      <c r="FG6" s="237"/>
-      <c r="FH6" s="237"/>
-      <c r="FI6" s="237"/>
-      <c r="FJ6" s="237"/>
-      <c r="FK6" s="237"/>
-      <c r="FL6" s="237"/>
-      <c r="FM6" s="237"/>
-      <c r="FN6" s="237"/>
-      <c r="FO6" s="237"/>
-      <c r="FP6" s="237"/>
-      <c r="FQ6" s="237"/>
-      <c r="FR6" s="237"/>
-      <c r="FS6" s="237"/>
-      <c r="FT6" s="237"/>
-      <c r="FU6" s="237"/>
-      <c r="FV6" s="237"/>
-      <c r="FW6" s="237"/>
-      <c r="FX6" s="237"/>
-      <c r="FY6" s="237"/>
-      <c r="FZ6" s="238"/>
-      <c r="GA6" s="232">
+      <c r="EX6" s="242"/>
+      <c r="EY6" s="242"/>
+      <c r="EZ6" s="242"/>
+      <c r="FA6" s="242"/>
+      <c r="FB6" s="242"/>
+      <c r="FC6" s="242"/>
+      <c r="FD6" s="242"/>
+      <c r="FE6" s="242"/>
+      <c r="FF6" s="242"/>
+      <c r="FG6" s="242"/>
+      <c r="FH6" s="242"/>
+      <c r="FI6" s="242"/>
+      <c r="FJ6" s="242"/>
+      <c r="FK6" s="242"/>
+      <c r="FL6" s="242"/>
+      <c r="FM6" s="242"/>
+      <c r="FN6" s="242"/>
+      <c r="FO6" s="242"/>
+      <c r="FP6" s="242"/>
+      <c r="FQ6" s="242"/>
+      <c r="FR6" s="242"/>
+      <c r="FS6" s="242"/>
+      <c r="FT6" s="242"/>
+      <c r="FU6" s="242"/>
+      <c r="FV6" s="242"/>
+      <c r="FW6" s="242"/>
+      <c r="FX6" s="242"/>
+      <c r="FY6" s="242"/>
+      <c r="FZ6" s="243"/>
+      <c r="GA6" s="237">
         <v>7</v>
       </c>
-      <c r="GB6" s="232"/>
-      <c r="GC6" s="232"/>
-      <c r="GD6" s="232"/>
-      <c r="GE6" s="232"/>
-      <c r="GF6" s="232"/>
-      <c r="GG6" s="232"/>
-      <c r="GH6" s="232"/>
-      <c r="GI6" s="232"/>
-      <c r="GJ6" s="232"/>
-      <c r="GK6" s="232"/>
-      <c r="GL6" s="232"/>
-      <c r="GM6" s="232"/>
-      <c r="GN6" s="232"/>
-      <c r="GO6" s="232"/>
-      <c r="GP6" s="232"/>
-      <c r="GQ6" s="232"/>
-      <c r="GR6" s="232"/>
-      <c r="GS6" s="232"/>
-      <c r="GT6" s="232"/>
-      <c r="GU6" s="232"/>
-      <c r="GV6" s="232"/>
-      <c r="GW6" s="232"/>
-      <c r="GX6" s="232"/>
-      <c r="GY6" s="232"/>
-      <c r="GZ6" s="232"/>
-      <c r="HA6" s="232"/>
-      <c r="HB6" s="232"/>
-      <c r="HC6" s="232"/>
-      <c r="HD6" s="232"/>
-      <c r="HE6" s="233"/>
-      <c r="HF6" s="232">
+      <c r="GB6" s="237"/>
+      <c r="GC6" s="237"/>
+      <c r="GD6" s="237"/>
+      <c r="GE6" s="237"/>
+      <c r="GF6" s="237"/>
+      <c r="GG6" s="237"/>
+      <c r="GH6" s="237"/>
+      <c r="GI6" s="237"/>
+      <c r="GJ6" s="237"/>
+      <c r="GK6" s="237"/>
+      <c r="GL6" s="237"/>
+      <c r="GM6" s="237"/>
+      <c r="GN6" s="237"/>
+      <c r="GO6" s="237"/>
+      <c r="GP6" s="237"/>
+      <c r="GQ6" s="237"/>
+      <c r="GR6" s="237"/>
+      <c r="GS6" s="237"/>
+      <c r="GT6" s="237"/>
+      <c r="GU6" s="237"/>
+      <c r="GV6" s="237"/>
+      <c r="GW6" s="237"/>
+      <c r="GX6" s="237"/>
+      <c r="GY6" s="237"/>
+      <c r="GZ6" s="237"/>
+      <c r="HA6" s="237"/>
+      <c r="HB6" s="237"/>
+      <c r="HC6" s="237"/>
+      <c r="HD6" s="237"/>
+      <c r="HE6" s="238"/>
+      <c r="HF6" s="237">
         <v>8</v>
       </c>
-      <c r="HG6" s="232"/>
-      <c r="HH6" s="232"/>
-      <c r="HI6" s="232"/>
-      <c r="HJ6" s="232"/>
-      <c r="HK6" s="232"/>
-      <c r="HL6" s="232"/>
-      <c r="HM6" s="232"/>
-      <c r="HN6" s="232"/>
-      <c r="HO6" s="232"/>
-      <c r="HP6" s="232"/>
-      <c r="HQ6" s="232"/>
-      <c r="HR6" s="232"/>
-      <c r="HS6" s="232"/>
-      <c r="HT6" s="232"/>
-      <c r="HU6" s="232"/>
-      <c r="HV6" s="232"/>
-      <c r="HW6" s="232"/>
-      <c r="HX6" s="232"/>
-      <c r="HY6" s="232"/>
-      <c r="HZ6" s="232"/>
-      <c r="IA6" s="232"/>
-      <c r="IB6" s="232"/>
-      <c r="IC6" s="232"/>
-      <c r="ID6" s="232"/>
-      <c r="IE6" s="232"/>
-      <c r="IF6" s="232"/>
-      <c r="IG6" s="232"/>
-      <c r="IH6" s="232"/>
-      <c r="II6" s="232"/>
-      <c r="IJ6" s="233"/>
-      <c r="IK6" s="236">
+      <c r="HG6" s="237"/>
+      <c r="HH6" s="237"/>
+      <c r="HI6" s="237"/>
+      <c r="HJ6" s="237"/>
+      <c r="HK6" s="237"/>
+      <c r="HL6" s="237"/>
+      <c r="HM6" s="237"/>
+      <c r="HN6" s="237"/>
+      <c r="HO6" s="237"/>
+      <c r="HP6" s="237"/>
+      <c r="HQ6" s="237"/>
+      <c r="HR6" s="237"/>
+      <c r="HS6" s="237"/>
+      <c r="HT6" s="237"/>
+      <c r="HU6" s="237"/>
+      <c r="HV6" s="237"/>
+      <c r="HW6" s="237"/>
+      <c r="HX6" s="237"/>
+      <c r="HY6" s="237"/>
+      <c r="HZ6" s="237"/>
+      <c r="IA6" s="237"/>
+      <c r="IB6" s="237"/>
+      <c r="IC6" s="237"/>
+      <c r="ID6" s="237"/>
+      <c r="IE6" s="237"/>
+      <c r="IF6" s="237"/>
+      <c r="IG6" s="237"/>
+      <c r="IH6" s="237"/>
+      <c r="II6" s="237"/>
+      <c r="IJ6" s="238"/>
+      <c r="IK6" s="241">
         <v>9</v>
       </c>
-      <c r="IL6" s="237"/>
-      <c r="IM6" s="237"/>
-      <c r="IN6" s="237"/>
-      <c r="IO6" s="237"/>
-      <c r="IP6" s="237"/>
-      <c r="IQ6" s="237"/>
-      <c r="IR6" s="237"/>
-      <c r="IS6" s="237"/>
-      <c r="IT6" s="237"/>
-      <c r="IU6" s="237"/>
-      <c r="IV6" s="237"/>
-      <c r="IW6" s="237"/>
-      <c r="IX6" s="237"/>
-      <c r="IY6" s="237"/>
-      <c r="IZ6" s="237"/>
-      <c r="JA6" s="237"/>
-      <c r="JB6" s="237"/>
-      <c r="JC6" s="237"/>
-      <c r="JD6" s="237"/>
-      <c r="JE6" s="237"/>
-      <c r="JF6" s="237"/>
-      <c r="JG6" s="237"/>
-      <c r="JH6" s="237"/>
-      <c r="JI6" s="237"/>
-      <c r="JJ6" s="237"/>
-      <c r="JK6" s="237"/>
-      <c r="JL6" s="237"/>
-      <c r="JM6" s="237"/>
-      <c r="JN6" s="238"/>
-      <c r="JO6" s="232">
+      <c r="IL6" s="242"/>
+      <c r="IM6" s="242"/>
+      <c r="IN6" s="242"/>
+      <c r="IO6" s="242"/>
+      <c r="IP6" s="242"/>
+      <c r="IQ6" s="242"/>
+      <c r="IR6" s="242"/>
+      <c r="IS6" s="242"/>
+      <c r="IT6" s="242"/>
+      <c r="IU6" s="242"/>
+      <c r="IV6" s="242"/>
+      <c r="IW6" s="242"/>
+      <c r="IX6" s="242"/>
+      <c r="IY6" s="242"/>
+      <c r="IZ6" s="242"/>
+      <c r="JA6" s="242"/>
+      <c r="JB6" s="242"/>
+      <c r="JC6" s="242"/>
+      <c r="JD6" s="242"/>
+      <c r="JE6" s="242"/>
+      <c r="JF6" s="242"/>
+      <c r="JG6" s="242"/>
+      <c r="JH6" s="242"/>
+      <c r="JI6" s="242"/>
+      <c r="JJ6" s="242"/>
+      <c r="JK6" s="242"/>
+      <c r="JL6" s="242"/>
+      <c r="JM6" s="242"/>
+      <c r="JN6" s="243"/>
+      <c r="JO6" s="237">
         <v>10</v>
       </c>
-      <c r="JP6" s="232"/>
-      <c r="JQ6" s="232"/>
-      <c r="JR6" s="232"/>
-      <c r="JS6" s="232"/>
-      <c r="JT6" s="232"/>
-      <c r="JU6" s="232"/>
-      <c r="JV6" s="232"/>
-      <c r="JW6" s="232"/>
-      <c r="JX6" s="232"/>
-      <c r="JY6" s="232"/>
-      <c r="JZ6" s="232"/>
-      <c r="KA6" s="232"/>
-      <c r="KB6" s="232"/>
-      <c r="KC6" s="232"/>
-      <c r="KD6" s="232"/>
-      <c r="KE6" s="232"/>
-      <c r="KF6" s="232"/>
-      <c r="KG6" s="232"/>
-      <c r="KH6" s="232"/>
-      <c r="KI6" s="232"/>
-      <c r="KJ6" s="232"/>
-      <c r="KK6" s="232"/>
-      <c r="KL6" s="232"/>
-      <c r="KM6" s="232"/>
-      <c r="KN6" s="232"/>
-      <c r="KO6" s="232"/>
-      <c r="KP6" s="232"/>
-      <c r="KQ6" s="232"/>
-      <c r="KR6" s="232"/>
-      <c r="KS6" s="233"/>
-      <c r="KT6" s="236">
+      <c r="JP6" s="237"/>
+      <c r="JQ6" s="237"/>
+      <c r="JR6" s="237"/>
+      <c r="JS6" s="237"/>
+      <c r="JT6" s="237"/>
+      <c r="JU6" s="237"/>
+      <c r="JV6" s="237"/>
+      <c r="JW6" s="237"/>
+      <c r="JX6" s="237"/>
+      <c r="JY6" s="237"/>
+      <c r="JZ6" s="237"/>
+      <c r="KA6" s="237"/>
+      <c r="KB6" s="237"/>
+      <c r="KC6" s="237"/>
+      <c r="KD6" s="237"/>
+      <c r="KE6" s="237"/>
+      <c r="KF6" s="237"/>
+      <c r="KG6" s="237"/>
+      <c r="KH6" s="237"/>
+      <c r="KI6" s="237"/>
+      <c r="KJ6" s="237"/>
+      <c r="KK6" s="237"/>
+      <c r="KL6" s="237"/>
+      <c r="KM6" s="237"/>
+      <c r="KN6" s="237"/>
+      <c r="KO6" s="237"/>
+      <c r="KP6" s="237"/>
+      <c r="KQ6" s="237"/>
+      <c r="KR6" s="237"/>
+      <c r="KS6" s="238"/>
+      <c r="KT6" s="241">
         <v>11</v>
       </c>
-      <c r="KU6" s="237"/>
-      <c r="KV6" s="237"/>
-      <c r="KW6" s="237"/>
-      <c r="KX6" s="237"/>
-      <c r="KY6" s="237"/>
-      <c r="KZ6" s="237"/>
-      <c r="LA6" s="237"/>
-      <c r="LB6" s="237"/>
-      <c r="LC6" s="237"/>
-      <c r="LD6" s="237"/>
-      <c r="LE6" s="237"/>
-      <c r="LF6" s="237"/>
-      <c r="LG6" s="237"/>
-      <c r="LH6" s="237"/>
-      <c r="LI6" s="237"/>
-      <c r="LJ6" s="237"/>
-      <c r="LK6" s="237"/>
-      <c r="LL6" s="237"/>
-      <c r="LM6" s="237"/>
-      <c r="LN6" s="237"/>
-      <c r="LO6" s="237"/>
-      <c r="LP6" s="237"/>
-      <c r="LQ6" s="237"/>
-      <c r="LR6" s="237"/>
-      <c r="LS6" s="237"/>
-      <c r="LT6" s="237"/>
-      <c r="LU6" s="237"/>
-      <c r="LV6" s="237"/>
-      <c r="LW6" s="238"/>
-      <c r="LX6" s="232">
+      <c r="KU6" s="242"/>
+      <c r="KV6" s="242"/>
+      <c r="KW6" s="242"/>
+      <c r="KX6" s="242"/>
+      <c r="KY6" s="242"/>
+      <c r="KZ6" s="242"/>
+      <c r="LA6" s="242"/>
+      <c r="LB6" s="242"/>
+      <c r="LC6" s="242"/>
+      <c r="LD6" s="242"/>
+      <c r="LE6" s="242"/>
+      <c r="LF6" s="242"/>
+      <c r="LG6" s="242"/>
+      <c r="LH6" s="242"/>
+      <c r="LI6" s="242"/>
+      <c r="LJ6" s="242"/>
+      <c r="LK6" s="242"/>
+      <c r="LL6" s="242"/>
+      <c r="LM6" s="242"/>
+      <c r="LN6" s="242"/>
+      <c r="LO6" s="242"/>
+      <c r="LP6" s="242"/>
+      <c r="LQ6" s="242"/>
+      <c r="LR6" s="242"/>
+      <c r="LS6" s="242"/>
+      <c r="LT6" s="242"/>
+      <c r="LU6" s="242"/>
+      <c r="LV6" s="242"/>
+      <c r="LW6" s="243"/>
+      <c r="LX6" s="237">
         <v>12</v>
       </c>
-      <c r="LY6" s="232"/>
-      <c r="LZ6" s="232"/>
-      <c r="MA6" s="232"/>
-      <c r="MB6" s="232"/>
-      <c r="MC6" s="232"/>
-      <c r="MD6" s="232"/>
-      <c r="ME6" s="232"/>
-      <c r="MF6" s="232"/>
-      <c r="MG6" s="232"/>
-      <c r="MH6" s="232"/>
-      <c r="MI6" s="232"/>
-      <c r="MJ6" s="232"/>
-      <c r="MK6" s="232"/>
-      <c r="ML6" s="232"/>
-      <c r="MM6" s="232"/>
-      <c r="MN6" s="232"/>
-      <c r="MO6" s="232"/>
-      <c r="MP6" s="232"/>
-      <c r="MQ6" s="232"/>
-      <c r="MR6" s="232"/>
-      <c r="MS6" s="232"/>
-      <c r="MT6" s="232"/>
-      <c r="MU6" s="232"/>
-      <c r="MV6" s="232"/>
-      <c r="MW6" s="232"/>
-      <c r="MX6" s="232"/>
-      <c r="MY6" s="232"/>
-      <c r="MZ6" s="232"/>
-      <c r="NA6" s="232"/>
-      <c r="NB6" s="233"/>
+      <c r="LY6" s="237"/>
+      <c r="LZ6" s="237"/>
+      <c r="MA6" s="237"/>
+      <c r="MB6" s="237"/>
+      <c r="MC6" s="237"/>
+      <c r="MD6" s="237"/>
+      <c r="ME6" s="237"/>
+      <c r="MF6" s="237"/>
+      <c r="MG6" s="237"/>
+      <c r="MH6" s="237"/>
+      <c r="MI6" s="237"/>
+      <c r="MJ6" s="237"/>
+      <c r="MK6" s="237"/>
+      <c r="ML6" s="237"/>
+      <c r="MM6" s="237"/>
+      <c r="MN6" s="237"/>
+      <c r="MO6" s="237"/>
+      <c r="MP6" s="237"/>
+      <c r="MQ6" s="237"/>
+      <c r="MR6" s="237"/>
+      <c r="MS6" s="237"/>
+      <c r="MT6" s="237"/>
+      <c r="MU6" s="237"/>
+      <c r="MV6" s="237"/>
+      <c r="MW6" s="237"/>
+      <c r="MX6" s="237"/>
+      <c r="MY6" s="237"/>
+      <c r="MZ6" s="237"/>
+      <c r="NA6" s="237"/>
+      <c r="NB6" s="238"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -18181,7 +18188,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="239" t="s">
+      <c r="A8" s="244" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -18569,7 +18576,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="239"/>
+      <c r="A9" s="244"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -18949,7 +18956,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="239"/>
+      <c r="A10" s="244"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -19329,7 +19336,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="239"/>
+      <c r="A11" s="244"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -19705,7 +19712,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="239"/>
+      <c r="A12" s="244"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -20079,7 +20086,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="239"/>
+      <c r="A13" s="244"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -20449,7 +20456,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="239"/>
+      <c r="A14" s="244"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -20819,7 +20826,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="239" t="s">
+      <c r="A15" s="244" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -21203,7 +21210,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="239"/>
+      <c r="A16" s="244"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -21583,7 +21590,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="239"/>
+      <c r="A17" s="244"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -21959,7 +21966,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="239"/>
+      <c r="A18" s="244"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -22335,7 +22342,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="239"/>
+      <c r="A19" s="244"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -22705,7 +22712,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="239" t="s">
+      <c r="A20" s="244" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -23083,7 +23090,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="239"/>
+      <c r="A21" s="244"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -23457,7 +23464,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="239"/>
+      <c r="A22" s="244"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -23829,7 +23836,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="239"/>
+      <c r="A23" s="244"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -24205,7 +24212,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="239"/>
+      <c r="A24" s="244"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -24573,7 +24580,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="240" t="s">
+      <c r="A25" s="245" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="75"/>
@@ -24949,7 +24956,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="239"/>
+      <c r="A26" s="244"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -25321,7 +25328,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="239"/>
+      <c r="A27" s="244"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -25695,7 +25702,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="239"/>
+      <c r="A28" s="244"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -26067,7 +26074,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="239"/>
+      <c r="A29" s="244"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -26437,7 +26444,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="240" t="s">
+      <c r="A30" s="245" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -26809,7 +26816,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="239"/>
+      <c r="A31" s="244"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -27183,7 +27190,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="239"/>
+      <c r="A32" s="244"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -27557,7 +27564,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="239"/>
+      <c r="A33" s="244"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -27927,7 +27934,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="239"/>
+      <c r="A34" s="244"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -28295,7 +28302,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="239" t="s">
+      <c r="A35" s="244" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -28677,7 +28684,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="239"/>
+      <c r="A36" s="244"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -29049,7 +29056,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="239"/>
+      <c r="A37" s="244"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -29427,7 +29434,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="239"/>
+      <c r="A38" s="244"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -29797,7 +29804,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="239"/>
+      <c r="A39" s="244"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -30169,7 +30176,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="239" t="s">
+      <c r="A40" s="244" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -30547,7 +30554,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="239"/>
+      <c r="A41" s="244"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -30921,7 +30928,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="239"/>
+      <c r="A42" s="244"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -31293,7 +31300,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="239"/>
+      <c r="A43" s="244"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -31663,7 +31670,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="239"/>
+      <c r="A44" s="244"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -32031,7 +32038,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="239" t="s">
+      <c r="A45" s="244" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -32411,7 +32418,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="239"/>
+      <c r="A46" s="244"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -32781,7 +32788,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="239"/>
+      <c r="A47" s="244"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -33157,7 +33164,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="239"/>
+      <c r="A48" s="244"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -33527,7 +33534,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="239"/>
+      <c r="A49" s="244"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -33901,7 +33908,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="239" t="s">
+      <c r="A50" s="244" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -34283,7 +34290,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="239"/>
+      <c r="A51" s="244"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -34661,7 +34668,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="239"/>
+      <c r="A52" s="244"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -35033,7 +35040,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="239"/>
+      <c r="A53" s="244"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -35403,7 +35410,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="239"/>
+      <c r="A54" s="244"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -35789,11 +35796,6 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="GA6:HE6"/>
-    <mergeCell ref="HF6:IJ6"/>
-    <mergeCell ref="IK6:JN6"/>
-    <mergeCell ref="JO6:KS6"/>
-    <mergeCell ref="KT6:LW6"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A15:A19"/>
@@ -35810,6 +35812,11 @@
     <mergeCell ref="BI6:CM6"/>
     <mergeCell ref="CN6:DQ6"/>
     <mergeCell ref="DR6:EV6"/>
+    <mergeCell ref="GA6:HE6"/>
+    <mergeCell ref="HF6:IJ6"/>
+    <mergeCell ref="IK6:JN6"/>
+    <mergeCell ref="JO6:KS6"/>
+    <mergeCell ref="KT6:LW6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35862,395 +35869,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="235">
+      <c r="B6" s="240">
         <v>1</v>
       </c>
-      <c r="C6" s="232"/>
-      <c r="D6" s="232"/>
-      <c r="E6" s="232"/>
-      <c r="F6" s="232"/>
-      <c r="G6" s="232"/>
-      <c r="H6" s="232"/>
-      <c r="I6" s="232"/>
-      <c r="J6" s="232"/>
-      <c r="K6" s="232"/>
-      <c r="L6" s="232"/>
-      <c r="M6" s="232"/>
-      <c r="N6" s="232"/>
-      <c r="O6" s="232"/>
-      <c r="P6" s="232"/>
-      <c r="Q6" s="232"/>
-      <c r="R6" s="232"/>
-      <c r="S6" s="232"/>
-      <c r="T6" s="232"/>
-      <c r="U6" s="232"/>
-      <c r="V6" s="232"/>
-      <c r="W6" s="232"/>
-      <c r="X6" s="232"/>
-      <c r="Y6" s="232"/>
-      <c r="Z6" s="232"/>
-      <c r="AA6" s="232"/>
-      <c r="AB6" s="232"/>
-      <c r="AC6" s="232"/>
-      <c r="AD6" s="232"/>
-      <c r="AE6" s="232"/>
-      <c r="AF6" s="232"/>
-      <c r="AG6" s="235">
+      <c r="C6" s="237"/>
+      <c r="D6" s="237"/>
+      <c r="E6" s="237"/>
+      <c r="F6" s="237"/>
+      <c r="G6" s="237"/>
+      <c r="H6" s="237"/>
+      <c r="I6" s="237"/>
+      <c r="J6" s="237"/>
+      <c r="K6" s="237"/>
+      <c r="L6" s="237"/>
+      <c r="M6" s="237"/>
+      <c r="N6" s="237"/>
+      <c r="O6" s="237"/>
+      <c r="P6" s="237"/>
+      <c r="Q6" s="237"/>
+      <c r="R6" s="237"/>
+      <c r="S6" s="237"/>
+      <c r="T6" s="237"/>
+      <c r="U6" s="237"/>
+      <c r="V6" s="237"/>
+      <c r="W6" s="237"/>
+      <c r="X6" s="237"/>
+      <c r="Y6" s="237"/>
+      <c r="Z6" s="237"/>
+      <c r="AA6" s="237"/>
+      <c r="AB6" s="237"/>
+      <c r="AC6" s="237"/>
+      <c r="AD6" s="237"/>
+      <c r="AE6" s="237"/>
+      <c r="AF6" s="237"/>
+      <c r="AG6" s="240">
         <v>2</v>
       </c>
-      <c r="AH6" s="232"/>
-      <c r="AI6" s="232"/>
-      <c r="AJ6" s="232"/>
-      <c r="AK6" s="232"/>
-      <c r="AL6" s="232"/>
-      <c r="AM6" s="232"/>
-      <c r="AN6" s="232"/>
-      <c r="AO6" s="232"/>
-      <c r="AP6" s="232"/>
-      <c r="AQ6" s="232"/>
-      <c r="AR6" s="232"/>
-      <c r="AS6" s="232"/>
-      <c r="AT6" s="232"/>
-      <c r="AU6" s="232"/>
-      <c r="AV6" s="232"/>
-      <c r="AW6" s="232"/>
-      <c r="AX6" s="232"/>
-      <c r="AY6" s="232"/>
-      <c r="AZ6" s="232"/>
-      <c r="BA6" s="232"/>
-      <c r="BB6" s="232"/>
-      <c r="BC6" s="232"/>
-      <c r="BD6" s="232"/>
-      <c r="BE6" s="232"/>
-      <c r="BF6" s="232"/>
-      <c r="BG6" s="232"/>
-      <c r="BH6" s="233"/>
-      <c r="BI6" s="232">
+      <c r="AH6" s="237"/>
+      <c r="AI6" s="237"/>
+      <c r="AJ6" s="237"/>
+      <c r="AK6" s="237"/>
+      <c r="AL6" s="237"/>
+      <c r="AM6" s="237"/>
+      <c r="AN6" s="237"/>
+      <c r="AO6" s="237"/>
+      <c r="AP6" s="237"/>
+      <c r="AQ6" s="237"/>
+      <c r="AR6" s="237"/>
+      <c r="AS6" s="237"/>
+      <c r="AT6" s="237"/>
+      <c r="AU6" s="237"/>
+      <c r="AV6" s="237"/>
+      <c r="AW6" s="237"/>
+      <c r="AX6" s="237"/>
+      <c r="AY6" s="237"/>
+      <c r="AZ6" s="237"/>
+      <c r="BA6" s="237"/>
+      <c r="BB6" s="237"/>
+      <c r="BC6" s="237"/>
+      <c r="BD6" s="237"/>
+      <c r="BE6" s="237"/>
+      <c r="BF6" s="237"/>
+      <c r="BG6" s="237"/>
+      <c r="BH6" s="238"/>
+      <c r="BI6" s="237">
         <v>3</v>
       </c>
-      <c r="BJ6" s="232"/>
-      <c r="BK6" s="232"/>
-      <c r="BL6" s="232"/>
-      <c r="BM6" s="232"/>
-      <c r="BN6" s="232"/>
-      <c r="BO6" s="232"/>
-      <c r="BP6" s="232"/>
-      <c r="BQ6" s="232"/>
-      <c r="BR6" s="232"/>
-      <c r="BS6" s="232"/>
-      <c r="BT6" s="232"/>
-      <c r="BU6" s="232"/>
-      <c r="BV6" s="232"/>
-      <c r="BW6" s="232"/>
-      <c r="BX6" s="232"/>
-      <c r="BY6" s="232"/>
-      <c r="BZ6" s="232"/>
-      <c r="CA6" s="232"/>
-      <c r="CB6" s="232"/>
-      <c r="CC6" s="232"/>
-      <c r="CD6" s="232"/>
-      <c r="CE6" s="232"/>
-      <c r="CF6" s="232"/>
-      <c r="CG6" s="232"/>
-      <c r="CH6" s="232"/>
-      <c r="CI6" s="232"/>
-      <c r="CJ6" s="232"/>
-      <c r="CK6" s="232"/>
-      <c r="CL6" s="232"/>
-      <c r="CM6" s="232"/>
-      <c r="CN6" s="236">
+      <c r="BJ6" s="237"/>
+      <c r="BK6" s="237"/>
+      <c r="BL6" s="237"/>
+      <c r="BM6" s="237"/>
+      <c r="BN6" s="237"/>
+      <c r="BO6" s="237"/>
+      <c r="BP6" s="237"/>
+      <c r="BQ6" s="237"/>
+      <c r="BR6" s="237"/>
+      <c r="BS6" s="237"/>
+      <c r="BT6" s="237"/>
+      <c r="BU6" s="237"/>
+      <c r="BV6" s="237"/>
+      <c r="BW6" s="237"/>
+      <c r="BX6" s="237"/>
+      <c r="BY6" s="237"/>
+      <c r="BZ6" s="237"/>
+      <c r="CA6" s="237"/>
+      <c r="CB6" s="237"/>
+      <c r="CC6" s="237"/>
+      <c r="CD6" s="237"/>
+      <c r="CE6" s="237"/>
+      <c r="CF6" s="237"/>
+      <c r="CG6" s="237"/>
+      <c r="CH6" s="237"/>
+      <c r="CI6" s="237"/>
+      <c r="CJ6" s="237"/>
+      <c r="CK6" s="237"/>
+      <c r="CL6" s="237"/>
+      <c r="CM6" s="237"/>
+      <c r="CN6" s="241">
         <v>4</v>
       </c>
-      <c r="CO6" s="237"/>
-      <c r="CP6" s="237"/>
-      <c r="CQ6" s="237"/>
-      <c r="CR6" s="237"/>
-      <c r="CS6" s="237"/>
-      <c r="CT6" s="237"/>
-      <c r="CU6" s="237"/>
-      <c r="CV6" s="237"/>
-      <c r="CW6" s="237"/>
-      <c r="CX6" s="237"/>
-      <c r="CY6" s="237"/>
-      <c r="CZ6" s="237"/>
-      <c r="DA6" s="237"/>
-      <c r="DB6" s="237"/>
-      <c r="DC6" s="237"/>
-      <c r="DD6" s="237"/>
-      <c r="DE6" s="237"/>
-      <c r="DF6" s="237"/>
-      <c r="DG6" s="237"/>
-      <c r="DH6" s="237"/>
-      <c r="DI6" s="237"/>
-      <c r="DJ6" s="237"/>
-      <c r="DK6" s="237"/>
-      <c r="DL6" s="237"/>
-      <c r="DM6" s="237"/>
-      <c r="DN6" s="237"/>
-      <c r="DO6" s="237"/>
-      <c r="DP6" s="237"/>
-      <c r="DQ6" s="238"/>
-      <c r="DR6" s="232">
+      <c r="CO6" s="242"/>
+      <c r="CP6" s="242"/>
+      <c r="CQ6" s="242"/>
+      <c r="CR6" s="242"/>
+      <c r="CS6" s="242"/>
+      <c r="CT6" s="242"/>
+      <c r="CU6" s="242"/>
+      <c r="CV6" s="242"/>
+      <c r="CW6" s="242"/>
+      <c r="CX6" s="242"/>
+      <c r="CY6" s="242"/>
+      <c r="CZ6" s="242"/>
+      <c r="DA6" s="242"/>
+      <c r="DB6" s="242"/>
+      <c r="DC6" s="242"/>
+      <c r="DD6" s="242"/>
+      <c r="DE6" s="242"/>
+      <c r="DF6" s="242"/>
+      <c r="DG6" s="242"/>
+      <c r="DH6" s="242"/>
+      <c r="DI6" s="242"/>
+      <c r="DJ6" s="242"/>
+      <c r="DK6" s="242"/>
+      <c r="DL6" s="242"/>
+      <c r="DM6" s="242"/>
+      <c r="DN6" s="242"/>
+      <c r="DO6" s="242"/>
+      <c r="DP6" s="242"/>
+      <c r="DQ6" s="243"/>
+      <c r="DR6" s="237">
         <v>5</v>
       </c>
-      <c r="DS6" s="232"/>
-      <c r="DT6" s="232"/>
-      <c r="DU6" s="232"/>
-      <c r="DV6" s="232"/>
-      <c r="DW6" s="232"/>
-      <c r="DX6" s="232"/>
-      <c r="DY6" s="232"/>
-      <c r="DZ6" s="232"/>
-      <c r="EA6" s="232"/>
-      <c r="EB6" s="232"/>
-      <c r="EC6" s="232"/>
-      <c r="ED6" s="232"/>
-      <c r="EE6" s="232"/>
-      <c r="EF6" s="232"/>
-      <c r="EG6" s="232"/>
-      <c r="EH6" s="232"/>
-      <c r="EI6" s="232"/>
-      <c r="EJ6" s="232"/>
-      <c r="EK6" s="232"/>
-      <c r="EL6" s="232"/>
-      <c r="EM6" s="232"/>
-      <c r="EN6" s="232"/>
-      <c r="EO6" s="232"/>
-      <c r="EP6" s="232"/>
-      <c r="EQ6" s="232"/>
-      <c r="ER6" s="232"/>
-      <c r="ES6" s="232"/>
-      <c r="ET6" s="232"/>
-      <c r="EU6" s="232"/>
-      <c r="EV6" s="233"/>
-      <c r="EW6" s="236">
+      <c r="DS6" s="237"/>
+      <c r="DT6" s="237"/>
+      <c r="DU6" s="237"/>
+      <c r="DV6" s="237"/>
+      <c r="DW6" s="237"/>
+      <c r="DX6" s="237"/>
+      <c r="DY6" s="237"/>
+      <c r="DZ6" s="237"/>
+      <c r="EA6" s="237"/>
+      <c r="EB6" s="237"/>
+      <c r="EC6" s="237"/>
+      <c r="ED6" s="237"/>
+      <c r="EE6" s="237"/>
+      <c r="EF6" s="237"/>
+      <c r="EG6" s="237"/>
+      <c r="EH6" s="237"/>
+      <c r="EI6" s="237"/>
+      <c r="EJ6" s="237"/>
+      <c r="EK6" s="237"/>
+      <c r="EL6" s="237"/>
+      <c r="EM6" s="237"/>
+      <c r="EN6" s="237"/>
+      <c r="EO6" s="237"/>
+      <c r="EP6" s="237"/>
+      <c r="EQ6" s="237"/>
+      <c r="ER6" s="237"/>
+      <c r="ES6" s="237"/>
+      <c r="ET6" s="237"/>
+      <c r="EU6" s="237"/>
+      <c r="EV6" s="238"/>
+      <c r="EW6" s="241">
         <v>6</v>
       </c>
-      <c r="EX6" s="237"/>
-      <c r="EY6" s="237"/>
-      <c r="EZ6" s="237"/>
-      <c r="FA6" s="237"/>
-      <c r="FB6" s="237"/>
-      <c r="FC6" s="237"/>
-      <c r="FD6" s="237"/>
-      <c r="FE6" s="237"/>
-      <c r="FF6" s="237"/>
-      <c r="FG6" s="237"/>
-      <c r="FH6" s="237"/>
-      <c r="FI6" s="237"/>
-      <c r="FJ6" s="237"/>
-      <c r="FK6" s="237"/>
-      <c r="FL6" s="237"/>
-      <c r="FM6" s="237"/>
-      <c r="FN6" s="237"/>
-      <c r="FO6" s="237"/>
-      <c r="FP6" s="237"/>
-      <c r="FQ6" s="237"/>
-      <c r="FR6" s="237"/>
-      <c r="FS6" s="237"/>
-      <c r="FT6" s="237"/>
-      <c r="FU6" s="237"/>
-      <c r="FV6" s="237"/>
-      <c r="FW6" s="237"/>
-      <c r="FX6" s="237"/>
-      <c r="FY6" s="237"/>
-      <c r="FZ6" s="238"/>
-      <c r="GA6" s="232">
+      <c r="EX6" s="242"/>
+      <c r="EY6" s="242"/>
+      <c r="EZ6" s="242"/>
+      <c r="FA6" s="242"/>
+      <c r="FB6" s="242"/>
+      <c r="FC6" s="242"/>
+      <c r="FD6" s="242"/>
+      <c r="FE6" s="242"/>
+      <c r="FF6" s="242"/>
+      <c r="FG6" s="242"/>
+      <c r="FH6" s="242"/>
+      <c r="FI6" s="242"/>
+      <c r="FJ6" s="242"/>
+      <c r="FK6" s="242"/>
+      <c r="FL6" s="242"/>
+      <c r="FM6" s="242"/>
+      <c r="FN6" s="242"/>
+      <c r="FO6" s="242"/>
+      <c r="FP6" s="242"/>
+      <c r="FQ6" s="242"/>
+      <c r="FR6" s="242"/>
+      <c r="FS6" s="242"/>
+      <c r="FT6" s="242"/>
+      <c r="FU6" s="242"/>
+      <c r="FV6" s="242"/>
+      <c r="FW6" s="242"/>
+      <c r="FX6" s="242"/>
+      <c r="FY6" s="242"/>
+      <c r="FZ6" s="243"/>
+      <c r="GA6" s="237">
         <v>7</v>
       </c>
-      <c r="GB6" s="232"/>
-      <c r="GC6" s="232"/>
-      <c r="GD6" s="232"/>
-      <c r="GE6" s="232"/>
-      <c r="GF6" s="232"/>
-      <c r="GG6" s="232"/>
-      <c r="GH6" s="232"/>
-      <c r="GI6" s="232"/>
-      <c r="GJ6" s="232"/>
-      <c r="GK6" s="232"/>
-      <c r="GL6" s="232"/>
-      <c r="GM6" s="232"/>
-      <c r="GN6" s="232"/>
-      <c r="GO6" s="232"/>
-      <c r="GP6" s="232"/>
-      <c r="GQ6" s="232"/>
-      <c r="GR6" s="232"/>
-      <c r="GS6" s="232"/>
-      <c r="GT6" s="232"/>
-      <c r="GU6" s="232"/>
-      <c r="GV6" s="232"/>
-      <c r="GW6" s="232"/>
-      <c r="GX6" s="232"/>
-      <c r="GY6" s="232"/>
-      <c r="GZ6" s="232"/>
-      <c r="HA6" s="232"/>
-      <c r="HB6" s="232"/>
-      <c r="HC6" s="232"/>
-      <c r="HD6" s="232"/>
-      <c r="HE6" s="233"/>
-      <c r="HF6" s="232">
+      <c r="GB6" s="237"/>
+      <c r="GC6" s="237"/>
+      <c r="GD6" s="237"/>
+      <c r="GE6" s="237"/>
+      <c r="GF6" s="237"/>
+      <c r="GG6" s="237"/>
+      <c r="GH6" s="237"/>
+      <c r="GI6" s="237"/>
+      <c r="GJ6" s="237"/>
+      <c r="GK6" s="237"/>
+      <c r="GL6" s="237"/>
+      <c r="GM6" s="237"/>
+      <c r="GN6" s="237"/>
+      <c r="GO6" s="237"/>
+      <c r="GP6" s="237"/>
+      <c r="GQ6" s="237"/>
+      <c r="GR6" s="237"/>
+      <c r="GS6" s="237"/>
+      <c r="GT6" s="237"/>
+      <c r="GU6" s="237"/>
+      <c r="GV6" s="237"/>
+      <c r="GW6" s="237"/>
+      <c r="GX6" s="237"/>
+      <c r="GY6" s="237"/>
+      <c r="GZ6" s="237"/>
+      <c r="HA6" s="237"/>
+      <c r="HB6" s="237"/>
+      <c r="HC6" s="237"/>
+      <c r="HD6" s="237"/>
+      <c r="HE6" s="238"/>
+      <c r="HF6" s="237">
         <v>8</v>
       </c>
-      <c r="HG6" s="232"/>
-      <c r="HH6" s="232"/>
-      <c r="HI6" s="232"/>
-      <c r="HJ6" s="232"/>
-      <c r="HK6" s="232"/>
-      <c r="HL6" s="232"/>
-      <c r="HM6" s="232"/>
-      <c r="HN6" s="232"/>
-      <c r="HO6" s="232"/>
-      <c r="HP6" s="232"/>
-      <c r="HQ6" s="232"/>
-      <c r="HR6" s="232"/>
-      <c r="HS6" s="232"/>
-      <c r="HT6" s="232"/>
-      <c r="HU6" s="232"/>
-      <c r="HV6" s="232"/>
-      <c r="HW6" s="232"/>
-      <c r="HX6" s="232"/>
-      <c r="HY6" s="232"/>
-      <c r="HZ6" s="232"/>
-      <c r="IA6" s="232"/>
-      <c r="IB6" s="232"/>
-      <c r="IC6" s="232"/>
-      <c r="ID6" s="232"/>
-      <c r="IE6" s="232"/>
-      <c r="IF6" s="232"/>
-      <c r="IG6" s="232"/>
-      <c r="IH6" s="232"/>
-      <c r="II6" s="232"/>
-      <c r="IJ6" s="233"/>
-      <c r="IK6" s="236">
+      <c r="HG6" s="237"/>
+      <c r="HH6" s="237"/>
+      <c r="HI6" s="237"/>
+      <c r="HJ6" s="237"/>
+      <c r="HK6" s="237"/>
+      <c r="HL6" s="237"/>
+      <c r="HM6" s="237"/>
+      <c r="HN6" s="237"/>
+      <c r="HO6" s="237"/>
+      <c r="HP6" s="237"/>
+      <c r="HQ6" s="237"/>
+      <c r="HR6" s="237"/>
+      <c r="HS6" s="237"/>
+      <c r="HT6" s="237"/>
+      <c r="HU6" s="237"/>
+      <c r="HV6" s="237"/>
+      <c r="HW6" s="237"/>
+      <c r="HX6" s="237"/>
+      <c r="HY6" s="237"/>
+      <c r="HZ6" s="237"/>
+      <c r="IA6" s="237"/>
+      <c r="IB6" s="237"/>
+      <c r="IC6" s="237"/>
+      <c r="ID6" s="237"/>
+      <c r="IE6" s="237"/>
+      <c r="IF6" s="237"/>
+      <c r="IG6" s="237"/>
+      <c r="IH6" s="237"/>
+      <c r="II6" s="237"/>
+      <c r="IJ6" s="238"/>
+      <c r="IK6" s="241">
         <v>9</v>
       </c>
-      <c r="IL6" s="237"/>
-      <c r="IM6" s="237"/>
-      <c r="IN6" s="237"/>
-      <c r="IO6" s="237"/>
-      <c r="IP6" s="237"/>
-      <c r="IQ6" s="237"/>
-      <c r="IR6" s="237"/>
-      <c r="IS6" s="237"/>
-      <c r="IT6" s="237"/>
-      <c r="IU6" s="237"/>
-      <c r="IV6" s="237"/>
-      <c r="IW6" s="237"/>
-      <c r="IX6" s="237"/>
-      <c r="IY6" s="237"/>
-      <c r="IZ6" s="237"/>
-      <c r="JA6" s="237"/>
-      <c r="JB6" s="237"/>
-      <c r="JC6" s="237"/>
-      <c r="JD6" s="237"/>
-      <c r="JE6" s="237"/>
-      <c r="JF6" s="237"/>
-      <c r="JG6" s="237"/>
-      <c r="JH6" s="237"/>
-      <c r="JI6" s="237"/>
-      <c r="JJ6" s="237"/>
-      <c r="JK6" s="237"/>
-      <c r="JL6" s="237"/>
-      <c r="JM6" s="237"/>
-      <c r="JN6" s="238"/>
-      <c r="JO6" s="232">
+      <c r="IL6" s="242"/>
+      <c r="IM6" s="242"/>
+      <c r="IN6" s="242"/>
+      <c r="IO6" s="242"/>
+      <c r="IP6" s="242"/>
+      <c r="IQ6" s="242"/>
+      <c r="IR6" s="242"/>
+      <c r="IS6" s="242"/>
+      <c r="IT6" s="242"/>
+      <c r="IU6" s="242"/>
+      <c r="IV6" s="242"/>
+      <c r="IW6" s="242"/>
+      <c r="IX6" s="242"/>
+      <c r="IY6" s="242"/>
+      <c r="IZ6" s="242"/>
+      <c r="JA6" s="242"/>
+      <c r="JB6" s="242"/>
+      <c r="JC6" s="242"/>
+      <c r="JD6" s="242"/>
+      <c r="JE6" s="242"/>
+      <c r="JF6" s="242"/>
+      <c r="JG6" s="242"/>
+      <c r="JH6" s="242"/>
+      <c r="JI6" s="242"/>
+      <c r="JJ6" s="242"/>
+      <c r="JK6" s="242"/>
+      <c r="JL6" s="242"/>
+      <c r="JM6" s="242"/>
+      <c r="JN6" s="243"/>
+      <c r="JO6" s="237">
         <v>10</v>
       </c>
-      <c r="JP6" s="232"/>
-      <c r="JQ6" s="232"/>
-      <c r="JR6" s="232"/>
-      <c r="JS6" s="232"/>
-      <c r="JT6" s="232"/>
-      <c r="JU6" s="232"/>
-      <c r="JV6" s="232"/>
-      <c r="JW6" s="232"/>
-      <c r="JX6" s="232"/>
-      <c r="JY6" s="232"/>
-      <c r="JZ6" s="232"/>
-      <c r="KA6" s="232"/>
-      <c r="KB6" s="232"/>
-      <c r="KC6" s="232"/>
-      <c r="KD6" s="232"/>
-      <c r="KE6" s="232"/>
-      <c r="KF6" s="232"/>
-      <c r="KG6" s="232"/>
-      <c r="KH6" s="232"/>
-      <c r="KI6" s="232"/>
-      <c r="KJ6" s="232"/>
-      <c r="KK6" s="232"/>
-      <c r="KL6" s="232"/>
-      <c r="KM6" s="232"/>
-      <c r="KN6" s="232"/>
-      <c r="KO6" s="232"/>
-      <c r="KP6" s="232"/>
-      <c r="KQ6" s="232"/>
-      <c r="KR6" s="232"/>
-      <c r="KS6" s="233"/>
-      <c r="KT6" s="236">
+      <c r="JP6" s="237"/>
+      <c r="JQ6" s="237"/>
+      <c r="JR6" s="237"/>
+      <c r="JS6" s="237"/>
+      <c r="JT6" s="237"/>
+      <c r="JU6" s="237"/>
+      <c r="JV6" s="237"/>
+      <c r="JW6" s="237"/>
+      <c r="JX6" s="237"/>
+      <c r="JY6" s="237"/>
+      <c r="JZ6" s="237"/>
+      <c r="KA6" s="237"/>
+      <c r="KB6" s="237"/>
+      <c r="KC6" s="237"/>
+      <c r="KD6" s="237"/>
+      <c r="KE6" s="237"/>
+      <c r="KF6" s="237"/>
+      <c r="KG6" s="237"/>
+      <c r="KH6" s="237"/>
+      <c r="KI6" s="237"/>
+      <c r="KJ6" s="237"/>
+      <c r="KK6" s="237"/>
+      <c r="KL6" s="237"/>
+      <c r="KM6" s="237"/>
+      <c r="KN6" s="237"/>
+      <c r="KO6" s="237"/>
+      <c r="KP6" s="237"/>
+      <c r="KQ6" s="237"/>
+      <c r="KR6" s="237"/>
+      <c r="KS6" s="238"/>
+      <c r="KT6" s="241">
         <v>11</v>
       </c>
-      <c r="KU6" s="237"/>
-      <c r="KV6" s="237"/>
-      <c r="KW6" s="237"/>
-      <c r="KX6" s="237"/>
-      <c r="KY6" s="237"/>
-      <c r="KZ6" s="237"/>
-      <c r="LA6" s="237"/>
-      <c r="LB6" s="237"/>
-      <c r="LC6" s="237"/>
-      <c r="LD6" s="237"/>
-      <c r="LE6" s="237"/>
-      <c r="LF6" s="237"/>
-      <c r="LG6" s="237"/>
-      <c r="LH6" s="237"/>
-      <c r="LI6" s="237"/>
-      <c r="LJ6" s="237"/>
-      <c r="LK6" s="237"/>
-      <c r="LL6" s="237"/>
-      <c r="LM6" s="237"/>
-      <c r="LN6" s="237"/>
-      <c r="LO6" s="237"/>
-      <c r="LP6" s="237"/>
-      <c r="LQ6" s="237"/>
-      <c r="LR6" s="237"/>
-      <c r="LS6" s="237"/>
-      <c r="LT6" s="237"/>
-      <c r="LU6" s="237"/>
-      <c r="LV6" s="237"/>
-      <c r="LW6" s="238"/>
-      <c r="LX6" s="232">
+      <c r="KU6" s="242"/>
+      <c r="KV6" s="242"/>
+      <c r="KW6" s="242"/>
+      <c r="KX6" s="242"/>
+      <c r="KY6" s="242"/>
+      <c r="KZ6" s="242"/>
+      <c r="LA6" s="242"/>
+      <c r="LB6" s="242"/>
+      <c r="LC6" s="242"/>
+      <c r="LD6" s="242"/>
+      <c r="LE6" s="242"/>
+      <c r="LF6" s="242"/>
+      <c r="LG6" s="242"/>
+      <c r="LH6" s="242"/>
+      <c r="LI6" s="242"/>
+      <c r="LJ6" s="242"/>
+      <c r="LK6" s="242"/>
+      <c r="LL6" s="242"/>
+      <c r="LM6" s="242"/>
+      <c r="LN6" s="242"/>
+      <c r="LO6" s="242"/>
+      <c r="LP6" s="242"/>
+      <c r="LQ6" s="242"/>
+      <c r="LR6" s="242"/>
+      <c r="LS6" s="242"/>
+      <c r="LT6" s="242"/>
+      <c r="LU6" s="242"/>
+      <c r="LV6" s="242"/>
+      <c r="LW6" s="243"/>
+      <c r="LX6" s="237">
         <v>12</v>
       </c>
-      <c r="LY6" s="232"/>
-      <c r="LZ6" s="232"/>
-      <c r="MA6" s="232"/>
-      <c r="MB6" s="232"/>
-      <c r="MC6" s="232"/>
-      <c r="MD6" s="232"/>
-      <c r="ME6" s="232"/>
-      <c r="MF6" s="232"/>
-      <c r="MG6" s="232"/>
-      <c r="MH6" s="232"/>
-      <c r="MI6" s="232"/>
-      <c r="MJ6" s="232"/>
-      <c r="MK6" s="232"/>
-      <c r="ML6" s="232"/>
-      <c r="MM6" s="232"/>
-      <c r="MN6" s="232"/>
-      <c r="MO6" s="232"/>
-      <c r="MP6" s="232"/>
-      <c r="MQ6" s="232"/>
-      <c r="MR6" s="232"/>
-      <c r="MS6" s="232"/>
-      <c r="MT6" s="232"/>
-      <c r="MU6" s="232"/>
-      <c r="MV6" s="232"/>
-      <c r="MW6" s="232"/>
-      <c r="MX6" s="232"/>
-      <c r="MY6" s="232"/>
-      <c r="MZ6" s="232"/>
-      <c r="NA6" s="232"/>
-      <c r="NB6" s="233"/>
+      <c r="LY6" s="237"/>
+      <c r="LZ6" s="237"/>
+      <c r="MA6" s="237"/>
+      <c r="MB6" s="237"/>
+      <c r="MC6" s="237"/>
+      <c r="MD6" s="237"/>
+      <c r="ME6" s="237"/>
+      <c r="MF6" s="237"/>
+      <c r="MG6" s="237"/>
+      <c r="MH6" s="237"/>
+      <c r="MI6" s="237"/>
+      <c r="MJ6" s="237"/>
+      <c r="MK6" s="237"/>
+      <c r="ML6" s="237"/>
+      <c r="MM6" s="237"/>
+      <c r="MN6" s="237"/>
+      <c r="MO6" s="237"/>
+      <c r="MP6" s="237"/>
+      <c r="MQ6" s="237"/>
+      <c r="MR6" s="237"/>
+      <c r="MS6" s="237"/>
+      <c r="MT6" s="237"/>
+      <c r="MU6" s="237"/>
+      <c r="MV6" s="237"/>
+      <c r="MW6" s="237"/>
+      <c r="MX6" s="237"/>
+      <c r="MY6" s="237"/>
+      <c r="MZ6" s="237"/>
+      <c r="NA6" s="237"/>
+      <c r="NB6" s="238"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -37351,7 +37358,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="239" t="s">
+      <c r="A8" s="244" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -37743,7 +37750,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="239"/>
+      <c r="A9" s="244"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -37892,7 +37899,7 @@
       <c r="EE9" s="28"/>
       <c r="EF9" s="30"/>
       <c r="EG9" s="30"/>
-      <c r="EH9" s="258" t="s">
+      <c r="EH9" s="228" t="s">
         <v>169</v>
       </c>
       <c r="EI9" s="30"/>
@@ -38125,7 +38132,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="239"/>
+      <c r="A10" s="244"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -38254,7 +38261,7 @@
       <c r="DK10" s="30"/>
       <c r="DL10" s="30"/>
       <c r="DM10" s="30"/>
-      <c r="DN10" s="258" t="s">
+      <c r="DN10" s="228" t="s">
         <v>132</v>
       </c>
       <c r="DO10" s="31"/>
@@ -38507,7 +38514,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="239"/>
+      <c r="A11" s="244"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -38883,7 +38890,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="239"/>
+      <c r="A12" s="244"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -39257,7 +39264,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="239"/>
+      <c r="A13" s="244"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -39627,7 +39634,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="239"/>
+      <c r="A14" s="244"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -39997,7 +40004,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="240" t="s">
+      <c r="A15" s="245" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="75"/>
@@ -40377,7 +40384,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="239"/>
+      <c r="A16" s="244"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -40749,7 +40756,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="239"/>
+      <c r="A17" s="244"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -41117,7 +41124,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="239"/>
+      <c r="A18" s="244"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -41487,7 +41494,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="239"/>
+      <c r="A19" s="244"/>
       <c r="B19" s="85"/>
       <c r="C19" s="71"/>
       <c r="D19" s="71"/>
@@ -41855,7 +41862,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="239" t="s">
+      <c r="A20" s="244" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="42"/>
@@ -42239,7 +42246,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="239"/>
+      <c r="A21" s="244"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -42616,7 +42623,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="239"/>
+      <c r="A22" s="244"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -42996,7 +43003,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="239"/>
+      <c r="A23" s="244"/>
       <c r="B23" s="24"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -43372,7 +43379,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="239"/>
+      <c r="A24" s="244"/>
       <c r="B24" s="26"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -43742,7 +43749,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="239" t="s">
+      <c r="A25" s="244" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="75"/>
@@ -44122,7 +44129,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="239"/>
+      <c r="A26" s="244"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -44498,7 +44505,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="239"/>
+      <c r="A27" s="244"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -44870,7 +44877,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="239"/>
+      <c r="A28" s="244"/>
       <c r="B28" s="24"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -45243,7 +45250,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="239"/>
+      <c r="A29" s="244"/>
       <c r="B29" s="91"/>
       <c r="C29" s="92"/>
       <c r="D29" s="92"/>
@@ -45613,7 +45620,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="240" t="s">
+      <c r="A30" s="245" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -45985,7 +45992,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="239"/>
+      <c r="A31" s="244"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -46359,7 +46366,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="239"/>
+      <c r="A32" s="244"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -46733,7 +46740,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="239"/>
+      <c r="A33" s="244"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -47103,7 +47110,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="239"/>
+      <c r="A34" s="244"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -47471,7 +47478,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="239" t="s">
+      <c r="A35" s="244" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -47853,7 +47860,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="239"/>
+      <c r="A36" s="244"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -48225,7 +48232,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="239"/>
+      <c r="A37" s="244"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -48601,7 +48608,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="239"/>
+      <c r="A38" s="244"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -48975,7 +48982,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="239"/>
+      <c r="A39" s="244"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -49347,7 +49354,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="239" t="s">
+      <c r="A40" s="244" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -49725,7 +49732,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="239"/>
+      <c r="A41" s="244"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -50101,7 +50108,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="239"/>
+      <c r="A42" s="244"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -50471,7 +50478,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="239"/>
+      <c r="A43" s="244"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -50841,7 +50848,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="239"/>
+      <c r="A44" s="244"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -51209,7 +51216,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="239" t="s">
+      <c r="A45" s="244" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -51589,7 +51596,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="239"/>
+      <c r="A46" s="244"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -51959,7 +51966,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="239"/>
+      <c r="A47" s="244"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -52335,7 +52342,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="239"/>
+      <c r="A48" s="244"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -52705,7 +52712,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="239"/>
+      <c r="A49" s="244"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -53079,7 +53086,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="239" t="s">
+      <c r="A50" s="244" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -53461,7 +53468,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="239"/>
+      <c r="A51" s="244"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -53839,7 +53846,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="239"/>
+      <c r="A52" s="244"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -54211,7 +54218,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="239"/>
+      <c r="A53" s="244"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -54581,7 +54588,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="239"/>
+      <c r="A54" s="244"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -54969,6 +54976,15 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A35:A39"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="B6:AF6"/>
     <mergeCell ref="AG6:BH6"/>
@@ -54981,15 +54997,6 @@
     <mergeCell ref="IK6:JN6"/>
     <mergeCell ref="JO6:KS6"/>
     <mergeCell ref="KT6:LW6"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="A35:A39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -55003,8 +55010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -55022,43 +55029,43 @@
   <sheetData>
     <row r="1" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="252" t="s">
+      <c r="B2" s="257" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="249" t="s">
+      <c r="C2" s="254" t="s">
         <v>161</v>
       </c>
-      <c r="D2" s="250"/>
-      <c r="E2" s="250"/>
-      <c r="F2" s="251"/>
-      <c r="G2" s="244" t="s">
+      <c r="D2" s="255"/>
+      <c r="E2" s="255"/>
+      <c r="F2" s="256"/>
+      <c r="G2" s="249" t="s">
         <v>126</v>
       </c>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="246"/>
+      <c r="H2" s="250"/>
+      <c r="I2" s="250"/>
+      <c r="J2" s="251"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="253"/>
-      <c r="C3" s="256" t="s">
+      <c r="B3" s="258"/>
+      <c r="C3" s="261" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="247"/>
-      <c r="E3" s="247" t="s">
+      <c r="D3" s="252"/>
+      <c r="E3" s="252" t="s">
         <v>159</v>
       </c>
-      <c r="F3" s="248"/>
-      <c r="G3" s="257" t="s">
+      <c r="F3" s="253"/>
+      <c r="G3" s="262" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="242"/>
-      <c r="I3" s="242" t="s">
+      <c r="H3" s="247"/>
+      <c r="I3" s="247" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="243"/>
+      <c r="J3" s="248"/>
     </row>
     <row r="4" spans="2:10" s="167" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="253"/>
+      <c r="B4" s="258"/>
       <c r="C4" s="185" t="s">
         <v>122</v>
       </c>
@@ -55093,7 +55100,7 @@
       <c r="D5" s="183"/>
       <c r="E5" s="183">
         <f>SUM(E6:E38)</f>
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="F5" s="184"/>
       <c r="G5" s="194">
@@ -55103,7 +55110,7 @@
       <c r="H5" s="195"/>
       <c r="I5" s="195">
         <f>SUM(I6:I38)</f>
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="J5" s="196"/>
     </row>
@@ -55129,7 +55136,7 @@
       <c r="J6" s="177"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="241">
+      <c r="B7" s="246">
         <v>43219</v>
       </c>
       <c r="C7" s="197">
@@ -55150,7 +55157,7 @@
       <c r="J7" s="203"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="241"/>
+      <c r="B8" s="246"/>
       <c r="C8" s="204"/>
       <c r="D8" s="205"/>
       <c r="E8" s="206"/>
@@ -55182,7 +55189,7 @@
       <c r="J9" s="177"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="241">
+      <c r="B10" s="246">
         <v>43221</v>
       </c>
       <c r="C10" s="211">
@@ -55203,7 +55210,7 @@
       <c r="J10" s="200"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="241"/>
+      <c r="B11" s="246"/>
       <c r="C11" s="213">
         <v>2</v>
       </c>
@@ -55218,7 +55225,7 @@
       <c r="J11" s="220"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="241"/>
+      <c r="B12" s="246"/>
       <c r="C12" s="213">
         <v>1</v>
       </c>
@@ -55233,7 +55240,7 @@
       <c r="J12" s="220"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="241"/>
+      <c r="B13" s="246"/>
       <c r="C13" s="221">
         <v>1</v>
       </c>
@@ -55248,7 +55255,7 @@
       <c r="J13" s="207"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="254">
+      <c r="B14" s="259">
         <v>43222</v>
       </c>
       <c r="C14" s="197">
@@ -55269,7 +55276,7 @@
       <c r="J14" s="200"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="255"/>
+      <c r="B15" s="260"/>
       <c r="C15" s="204">
         <v>0.5</v>
       </c>
@@ -55309,7 +55316,7 @@
       <c r="J16" s="180"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="254">
+      <c r="B17" s="259">
         <v>43226</v>
       </c>
       <c r="C17" s="197"/>
@@ -55334,7 +55341,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="255"/>
+      <c r="B18" s="260"/>
       <c r="C18" s="204"/>
       <c r="D18" s="205"/>
       <c r="E18" s="206"/>
@@ -55442,7 +55449,7 @@
       <c r="J23" s="177"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="241">
+      <c r="B24" s="246">
         <v>43235</v>
       </c>
       <c r="C24" s="197">
@@ -55463,7 +55470,7 @@
       <c r="J24" s="200"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="241"/>
+      <c r="B25" s="246"/>
       <c r="C25" s="204">
         <v>2</v>
       </c>
@@ -55482,7 +55489,7 @@
       <c r="J25" s="210"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="241">
+      <c r="B26" s="246">
         <v>43236</v>
       </c>
       <c r="C26" s="197">
@@ -55503,7 +55510,7 @@
       <c r="J26" s="200"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="241"/>
+      <c r="B27" s="246"/>
       <c r="C27" s="223">
         <v>0.5</v>
       </c>
@@ -55522,7 +55529,7 @@
       <c r="J27" s="226"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="241"/>
+      <c r="B28" s="246"/>
       <c r="C28" s="223">
         <v>3</v>
       </c>
@@ -55537,7 +55544,7 @@
       <c r="J28" s="226"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="241"/>
+      <c r="B29" s="246"/>
       <c r="C29" s="223">
         <v>2</v>
       </c>
@@ -55552,7 +55559,7 @@
       <c r="J29" s="226"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="241"/>
+      <c r="B30" s="246"/>
       <c r="C30" s="204">
         <v>1</v>
       </c>
@@ -55584,15 +55591,25 @@
       <c r="J31" s="177"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="179"/>
-      <c r="C32" s="176"/>
+      <c r="B32" s="179">
+        <v>43242</v>
+      </c>
+      <c r="C32" s="264"/>
       <c r="D32" s="188"/>
-      <c r="E32" s="186"/>
-      <c r="F32" s="177"/>
+      <c r="E32" s="186">
+        <v>3</v>
+      </c>
+      <c r="F32" s="177" t="s">
+        <v>183</v>
+      </c>
       <c r="G32" s="178"/>
       <c r="H32" s="188"/>
-      <c r="I32" s="186"/>
-      <c r="J32" s="177"/>
+      <c r="I32" s="186">
+        <v>0.5</v>
+      </c>
+      <c r="J32" s="177" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="179"/>
@@ -55704,7 +55721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
@@ -55715,19 +55732,19 @@
     <col min="4" max="4" width="52.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" s="260" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="261" t="s">
+    <row r="3" spans="2:4" s="230" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="231" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="261" t="s">
+      <c r="C3" s="231" t="s">
         <v>181</v>
       </c>
-      <c r="D3" s="261" t="s">
+      <c r="D3" s="231" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="262">
+      <c r="B4" s="263">
         <v>43237</v>
       </c>
       <c r="C4" s="190" t="s">
@@ -55736,35 +55753,35 @@
       <c r="D4" s="190"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="262"/>
+      <c r="B5" s="263"/>
       <c r="C5" s="190" t="s">
         <v>172</v>
       </c>
       <c r="D5" s="190"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="262"/>
+      <c r="B6" s="263"/>
       <c r="C6" s="190" t="s">
         <v>173</v>
       </c>
       <c r="D6" s="190"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="262"/>
+      <c r="B7" s="263"/>
       <c r="C7" s="190" t="s">
         <v>174</v>
       </c>
       <c r="D7" s="190"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="262"/>
+      <c r="B8" s="263"/>
       <c r="C8" s="190" t="s">
         <v>175</v>
       </c>
       <c r="D8" s="190"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="262"/>
+      <c r="B9" s="263"/>
       <c r="C9" s="190" t="s">
         <v>176</v>
       </c>
@@ -55773,8 +55790,8 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="262"/>
-      <c r="C10" s="263" t="s">
+      <c r="B10" s="263"/>
+      <c r="C10" s="232" t="s">
         <v>180</v>
       </c>
       <c r="D10" s="188" t="s">
@@ -55782,7 +55799,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="262"/>
+      <c r="B11" s="263"/>
       <c r="C11" s="190" t="s">
         <v>178</v>
       </c>
@@ -55791,19 +55808,19 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="259"/>
+      <c r="B12" s="229"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="259"/>
+      <c r="B13" s="229"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="259"/>
+      <c r="B14" s="229"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="259"/>
+      <c r="B15" s="229"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="259"/>
+      <c r="B16" s="229"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
5/23 Working time update
</commit_message>
<xml_diff>
--- a/Femto Project schedule V1.0.xlsx
+++ b/Femto Project schedule V1.0.xlsx
@@ -283,7 +283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="185">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1023,6 +1023,10 @@
   </si>
   <si>
     <t>GEN Main Sch CON 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GEN Main ADC, Power review</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2382,6 +2386,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2473,9 +2480,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -9390,167 +9394,167 @@
     </row>
     <row r="6" spans="1:152" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="240">
+      <c r="B6" s="241">
         <v>1</v>
       </c>
-      <c r="C6" s="237"/>
-      <c r="D6" s="237"/>
-      <c r="E6" s="237"/>
-      <c r="F6" s="237"/>
-      <c r="G6" s="237"/>
-      <c r="H6" s="237"/>
-      <c r="I6" s="237"/>
-      <c r="J6" s="237"/>
-      <c r="K6" s="237"/>
-      <c r="L6" s="237"/>
-      <c r="M6" s="237"/>
-      <c r="N6" s="237"/>
-      <c r="O6" s="237"/>
-      <c r="P6" s="237"/>
-      <c r="Q6" s="237"/>
-      <c r="R6" s="237"/>
-      <c r="S6" s="237"/>
-      <c r="T6" s="237"/>
-      <c r="U6" s="237"/>
-      <c r="V6" s="237"/>
-      <c r="W6" s="237"/>
-      <c r="X6" s="237"/>
-      <c r="Y6" s="237"/>
-      <c r="Z6" s="237"/>
-      <c r="AA6" s="237"/>
-      <c r="AB6" s="237"/>
-      <c r="AC6" s="237"/>
-      <c r="AD6" s="237"/>
-      <c r="AE6" s="237"/>
-      <c r="AF6" s="237"/>
-      <c r="AG6" s="240">
+      <c r="C6" s="238"/>
+      <c r="D6" s="238"/>
+      <c r="E6" s="238"/>
+      <c r="F6" s="238"/>
+      <c r="G6" s="238"/>
+      <c r="H6" s="238"/>
+      <c r="I6" s="238"/>
+      <c r="J6" s="238"/>
+      <c r="K6" s="238"/>
+      <c r="L6" s="238"/>
+      <c r="M6" s="238"/>
+      <c r="N6" s="238"/>
+      <c r="O6" s="238"/>
+      <c r="P6" s="238"/>
+      <c r="Q6" s="238"/>
+      <c r="R6" s="238"/>
+      <c r="S6" s="238"/>
+      <c r="T6" s="238"/>
+      <c r="U6" s="238"/>
+      <c r="V6" s="238"/>
+      <c r="W6" s="238"/>
+      <c r="X6" s="238"/>
+      <c r="Y6" s="238"/>
+      <c r="Z6" s="238"/>
+      <c r="AA6" s="238"/>
+      <c r="AB6" s="238"/>
+      <c r="AC6" s="238"/>
+      <c r="AD6" s="238"/>
+      <c r="AE6" s="238"/>
+      <c r="AF6" s="238"/>
+      <c r="AG6" s="241">
         <v>2</v>
       </c>
-      <c r="AH6" s="237"/>
-      <c r="AI6" s="237"/>
-      <c r="AJ6" s="237"/>
-      <c r="AK6" s="237"/>
-      <c r="AL6" s="237"/>
-      <c r="AM6" s="237"/>
-      <c r="AN6" s="237"/>
-      <c r="AO6" s="237"/>
-      <c r="AP6" s="237"/>
-      <c r="AQ6" s="237"/>
-      <c r="AR6" s="237"/>
-      <c r="AS6" s="237"/>
-      <c r="AT6" s="237"/>
-      <c r="AU6" s="237"/>
-      <c r="AV6" s="237"/>
-      <c r="AW6" s="237"/>
-      <c r="AX6" s="237"/>
-      <c r="AY6" s="237"/>
-      <c r="AZ6" s="237"/>
-      <c r="BA6" s="237"/>
-      <c r="BB6" s="237"/>
-      <c r="BC6" s="237"/>
-      <c r="BD6" s="237"/>
-      <c r="BE6" s="237"/>
-      <c r="BF6" s="237"/>
-      <c r="BG6" s="237"/>
-      <c r="BH6" s="238"/>
-      <c r="BI6" s="237">
+      <c r="AH6" s="238"/>
+      <c r="AI6" s="238"/>
+      <c r="AJ6" s="238"/>
+      <c r="AK6" s="238"/>
+      <c r="AL6" s="238"/>
+      <c r="AM6" s="238"/>
+      <c r="AN6" s="238"/>
+      <c r="AO6" s="238"/>
+      <c r="AP6" s="238"/>
+      <c r="AQ6" s="238"/>
+      <c r="AR6" s="238"/>
+      <c r="AS6" s="238"/>
+      <c r="AT6" s="238"/>
+      <c r="AU6" s="238"/>
+      <c r="AV6" s="238"/>
+      <c r="AW6" s="238"/>
+      <c r="AX6" s="238"/>
+      <c r="AY6" s="238"/>
+      <c r="AZ6" s="238"/>
+      <c r="BA6" s="238"/>
+      <c r="BB6" s="238"/>
+      <c r="BC6" s="238"/>
+      <c r="BD6" s="238"/>
+      <c r="BE6" s="238"/>
+      <c r="BF6" s="238"/>
+      <c r="BG6" s="238"/>
+      <c r="BH6" s="239"/>
+      <c r="BI6" s="238">
         <v>3</v>
       </c>
-      <c r="BJ6" s="237"/>
-      <c r="BK6" s="237"/>
-      <c r="BL6" s="237"/>
-      <c r="BM6" s="237"/>
-      <c r="BN6" s="237"/>
-      <c r="BO6" s="237"/>
-      <c r="BP6" s="237"/>
-      <c r="BQ6" s="237"/>
-      <c r="BR6" s="237"/>
-      <c r="BS6" s="237"/>
-      <c r="BT6" s="237"/>
-      <c r="BU6" s="237"/>
-      <c r="BV6" s="237"/>
-      <c r="BW6" s="237"/>
-      <c r="BX6" s="237"/>
-      <c r="BY6" s="237"/>
-      <c r="BZ6" s="237"/>
-      <c r="CA6" s="237"/>
-      <c r="CB6" s="237"/>
-      <c r="CC6" s="237"/>
-      <c r="CD6" s="237"/>
-      <c r="CE6" s="237"/>
-      <c r="CF6" s="237"/>
-      <c r="CG6" s="237"/>
-      <c r="CH6" s="237"/>
-      <c r="CI6" s="237"/>
-      <c r="CJ6" s="237"/>
-      <c r="CK6" s="237"/>
-      <c r="CL6" s="237"/>
-      <c r="CM6" s="237"/>
-      <c r="CN6" s="241">
+      <c r="BJ6" s="238"/>
+      <c r="BK6" s="238"/>
+      <c r="BL6" s="238"/>
+      <c r="BM6" s="238"/>
+      <c r="BN6" s="238"/>
+      <c r="BO6" s="238"/>
+      <c r="BP6" s="238"/>
+      <c r="BQ6" s="238"/>
+      <c r="BR6" s="238"/>
+      <c r="BS6" s="238"/>
+      <c r="BT6" s="238"/>
+      <c r="BU6" s="238"/>
+      <c r="BV6" s="238"/>
+      <c r="BW6" s="238"/>
+      <c r="BX6" s="238"/>
+      <c r="BY6" s="238"/>
+      <c r="BZ6" s="238"/>
+      <c r="CA6" s="238"/>
+      <c r="CB6" s="238"/>
+      <c r="CC6" s="238"/>
+      <c r="CD6" s="238"/>
+      <c r="CE6" s="238"/>
+      <c r="CF6" s="238"/>
+      <c r="CG6" s="238"/>
+      <c r="CH6" s="238"/>
+      <c r="CI6" s="238"/>
+      <c r="CJ6" s="238"/>
+      <c r="CK6" s="238"/>
+      <c r="CL6" s="238"/>
+      <c r="CM6" s="238"/>
+      <c r="CN6" s="242">
         <v>4</v>
       </c>
-      <c r="CO6" s="242"/>
-      <c r="CP6" s="242"/>
-      <c r="CQ6" s="242"/>
-      <c r="CR6" s="242"/>
-      <c r="CS6" s="242"/>
-      <c r="CT6" s="242"/>
-      <c r="CU6" s="242"/>
-      <c r="CV6" s="242"/>
-      <c r="CW6" s="242"/>
-      <c r="CX6" s="242"/>
-      <c r="CY6" s="242"/>
-      <c r="CZ6" s="242"/>
-      <c r="DA6" s="242"/>
-      <c r="DB6" s="242"/>
-      <c r="DC6" s="242"/>
-      <c r="DD6" s="242"/>
-      <c r="DE6" s="242"/>
-      <c r="DF6" s="242"/>
-      <c r="DG6" s="242"/>
-      <c r="DH6" s="242"/>
-      <c r="DI6" s="242"/>
-      <c r="DJ6" s="242"/>
-      <c r="DK6" s="242"/>
-      <c r="DL6" s="242"/>
-      <c r="DM6" s="242"/>
-      <c r="DN6" s="242"/>
-      <c r="DO6" s="242"/>
-      <c r="DP6" s="242"/>
-      <c r="DQ6" s="243"/>
-      <c r="DR6" s="237">
+      <c r="CO6" s="243"/>
+      <c r="CP6" s="243"/>
+      <c r="CQ6" s="243"/>
+      <c r="CR6" s="243"/>
+      <c r="CS6" s="243"/>
+      <c r="CT6" s="243"/>
+      <c r="CU6" s="243"/>
+      <c r="CV6" s="243"/>
+      <c r="CW6" s="243"/>
+      <c r="CX6" s="243"/>
+      <c r="CY6" s="243"/>
+      <c r="CZ6" s="243"/>
+      <c r="DA6" s="243"/>
+      <c r="DB6" s="243"/>
+      <c r="DC6" s="243"/>
+      <c r="DD6" s="243"/>
+      <c r="DE6" s="243"/>
+      <c r="DF6" s="243"/>
+      <c r="DG6" s="243"/>
+      <c r="DH6" s="243"/>
+      <c r="DI6" s="243"/>
+      <c r="DJ6" s="243"/>
+      <c r="DK6" s="243"/>
+      <c r="DL6" s="243"/>
+      <c r="DM6" s="243"/>
+      <c r="DN6" s="243"/>
+      <c r="DO6" s="243"/>
+      <c r="DP6" s="243"/>
+      <c r="DQ6" s="244"/>
+      <c r="DR6" s="238">
         <v>5</v>
       </c>
-      <c r="DS6" s="237"/>
-      <c r="DT6" s="237"/>
-      <c r="DU6" s="237"/>
-      <c r="DV6" s="237"/>
-      <c r="DW6" s="237"/>
-      <c r="DX6" s="237"/>
-      <c r="DY6" s="237"/>
-      <c r="DZ6" s="237"/>
-      <c r="EA6" s="237"/>
-      <c r="EB6" s="237"/>
-      <c r="EC6" s="237"/>
-      <c r="ED6" s="237"/>
-      <c r="EE6" s="237"/>
-      <c r="EF6" s="237"/>
-      <c r="EG6" s="237"/>
-      <c r="EH6" s="237"/>
-      <c r="EI6" s="237"/>
-      <c r="EJ6" s="237"/>
-      <c r="EK6" s="237"/>
-      <c r="EL6" s="237"/>
-      <c r="EM6" s="237"/>
-      <c r="EN6" s="237"/>
-      <c r="EO6" s="237"/>
-      <c r="EP6" s="237"/>
-      <c r="EQ6" s="237"/>
-      <c r="ER6" s="237"/>
-      <c r="ES6" s="237"/>
-      <c r="ET6" s="237"/>
-      <c r="EU6" s="237"/>
-      <c r="EV6" s="238"/>
+      <c r="DS6" s="238"/>
+      <c r="DT6" s="238"/>
+      <c r="DU6" s="238"/>
+      <c r="DV6" s="238"/>
+      <c r="DW6" s="238"/>
+      <c r="DX6" s="238"/>
+      <c r="DY6" s="238"/>
+      <c r="DZ6" s="238"/>
+      <c r="EA6" s="238"/>
+      <c r="EB6" s="238"/>
+      <c r="EC6" s="238"/>
+      <c r="ED6" s="238"/>
+      <c r="EE6" s="238"/>
+      <c r="EF6" s="238"/>
+      <c r="EG6" s="238"/>
+      <c r="EH6" s="238"/>
+      <c r="EI6" s="238"/>
+      <c r="EJ6" s="238"/>
+      <c r="EK6" s="238"/>
+      <c r="EL6" s="238"/>
+      <c r="EM6" s="238"/>
+      <c r="EN6" s="238"/>
+      <c r="EO6" s="238"/>
+      <c r="EP6" s="238"/>
+      <c r="EQ6" s="238"/>
+      <c r="ER6" s="238"/>
+      <c r="ES6" s="238"/>
+      <c r="ET6" s="238"/>
+      <c r="EU6" s="238"/>
+      <c r="EV6" s="239"/>
     </row>
     <row r="7" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -10009,7 +10013,7 @@
       </c>
     </row>
     <row r="8" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A8" s="234" t="s">
+      <c r="A8" s="235" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -10173,7 +10177,7 @@
       <c r="EV8" s="99"/>
     </row>
     <row r="9" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A9" s="234"/>
+      <c r="A9" s="235"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -10333,7 +10337,7 @@
       <c r="EV9" s="33"/>
     </row>
     <row r="10" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A10" s="234"/>
+      <c r="A10" s="235"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -10493,7 +10497,7 @@
       <c r="EV10" s="33"/>
     </row>
     <row r="11" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A11" s="234"/>
+      <c r="A11" s="235"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -10651,7 +10655,7 @@
       <c r="EV11" s="33"/>
     </row>
     <row r="12" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A12" s="234"/>
+      <c r="A12" s="235"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -10809,7 +10813,7 @@
       <c r="EV12" s="33"/>
     </row>
     <row r="13" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A13" s="234"/>
+      <c r="A13" s="235"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -10965,7 +10969,7 @@
       <c r="EV13" s="33"/>
     </row>
     <row r="14" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="239"/>
+      <c r="A14" s="240"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -11119,7 +11123,7 @@
       <c r="EV14" s="100"/>
     </row>
     <row r="15" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A15" s="236" t="s">
+      <c r="A15" s="237" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -11281,7 +11285,7 @@
       <c r="EV15" s="102"/>
     </row>
     <row r="16" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A16" s="234"/>
+      <c r="A16" s="235"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -11439,7 +11443,7 @@
       <c r="EV16" s="17"/>
     </row>
     <row r="17" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A17" s="234"/>
+      <c r="A17" s="235"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -11599,7 +11603,7 @@
       <c r="EV17" s="17"/>
     </row>
     <row r="18" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A18" s="234"/>
+      <c r="A18" s="235"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -11755,7 +11759,7 @@
       <c r="EV18" s="17"/>
     </row>
     <row r="19" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="234"/>
+      <c r="A19" s="235"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -11911,7 +11915,7 @@
       <c r="EV19" s="98"/>
     </row>
     <row r="20" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="236" t="s">
+      <c r="A20" s="237" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -12073,7 +12077,7 @@
       <c r="EV20" s="102"/>
     </row>
     <row r="21" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="234"/>
+      <c r="A21" s="235"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -12231,7 +12235,7 @@
       <c r="EV21" s="17"/>
     </row>
     <row r="22" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="234"/>
+      <c r="A22" s="235"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -12389,7 +12393,7 @@
       <c r="EV22" s="17"/>
     </row>
     <row r="23" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="234"/>
+      <c r="A23" s="235"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -12547,7 +12551,7 @@
       <c r="EV23" s="17"/>
     </row>
     <row r="24" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="235"/>
+      <c r="A24" s="236"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -12701,7 +12705,7 @@
       <c r="EV24" s="98"/>
     </row>
     <row r="25" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="236" t="s">
+      <c r="A25" s="237" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="75"/>
@@ -12857,7 +12861,7 @@
       <c r="EV25" s="102"/>
     </row>
     <row r="26" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="234"/>
+      <c r="A26" s="235"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -13011,7 +13015,7 @@
       <c r="EV26" s="17"/>
     </row>
     <row r="27" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="234"/>
+      <c r="A27" s="235"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -13165,7 +13169,7 @@
       <c r="EV27" s="17"/>
     </row>
     <row r="28" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="234"/>
+      <c r="A28" s="235"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -13319,7 +13323,7 @@
       <c r="EV28" s="17"/>
     </row>
     <row r="29" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="234"/>
+      <c r="A29" s="235"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -13473,7 +13477,7 @@
       <c r="EV29" s="98"/>
     </row>
     <row r="30" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="233" t="s">
+      <c r="A30" s="234" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="75"/>
@@ -13639,7 +13643,7 @@
       <c r="EV30" s="102"/>
     </row>
     <row r="31" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="234"/>
+      <c r="A31" s="235"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -13797,7 +13801,7 @@
       <c r="EV31" s="17"/>
     </row>
     <row r="32" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="234"/>
+      <c r="A32" s="235"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -13955,7 +13959,7 @@
       <c r="EV32" s="17"/>
     </row>
     <row r="33" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="234"/>
+      <c r="A33" s="235"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -14111,7 +14115,7 @@
       <c r="EV33" s="17"/>
     </row>
     <row r="34" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="235"/>
+      <c r="A34" s="236"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -14267,7 +14271,7 @@
       <c r="EV34" s="98"/>
     </row>
     <row r="35" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="234" t="s">
+      <c r="A35" s="235" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="75"/>
@@ -14425,7 +14429,7 @@
       <c r="EV35" s="102"/>
     </row>
     <row r="36" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="234"/>
+      <c r="A36" s="235"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -14581,7 +14585,7 @@
       <c r="EV36" s="17"/>
     </row>
     <row r="37" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="234"/>
+      <c r="A37" s="235"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -14735,7 +14739,7 @@
       <c r="EV37" s="17"/>
     </row>
     <row r="38" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="234"/>
+      <c r="A38" s="235"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -14889,7 +14893,7 @@
       <c r="EV38" s="17"/>
     </row>
     <row r="39" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="234"/>
+      <c r="A39" s="235"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -15043,7 +15047,7 @@
       <c r="EV39" s="98"/>
     </row>
     <row r="40" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="233" t="s">
+      <c r="A40" s="234" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="75"/>
@@ -15205,7 +15209,7 @@
       <c r="EV40" s="102"/>
     </row>
     <row r="41" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="234"/>
+      <c r="A41" s="235"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -15361,7 +15365,7 @@
       <c r="EV41" s="17"/>
     </row>
     <row r="42" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="234"/>
+      <c r="A42" s="235"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -15519,7 +15523,7 @@
       <c r="EV42" s="17"/>
     </row>
     <row r="43" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="234"/>
+      <c r="A43" s="235"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -15675,7 +15679,7 @@
       <c r="EV43" s="17"/>
     </row>
     <row r="44" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="235"/>
+      <c r="A44" s="236"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -15831,7 +15835,7 @@
       <c r="EV44" s="98"/>
     </row>
     <row r="45" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="234" t="s">
+      <c r="A45" s="235" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="75"/>
@@ -15993,7 +15997,7 @@
       <c r="EV45" s="102"/>
     </row>
     <row r="46" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="234"/>
+      <c r="A46" s="235"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -16149,7 +16153,7 @@
       <c r="EV46" s="17"/>
     </row>
     <row r="47" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="234"/>
+      <c r="A47" s="235"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -16307,7 +16311,7 @@
       <c r="EV47" s="17"/>
     </row>
     <row r="48" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="234"/>
+      <c r="A48" s="235"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -16463,7 +16467,7 @@
       <c r="EV48" s="17"/>
     </row>
     <row r="49" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="235"/>
+      <c r="A49" s="236"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -16699,395 +16703,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="240">
+      <c r="B6" s="241">
         <v>1</v>
       </c>
-      <c r="C6" s="237"/>
-      <c r="D6" s="237"/>
-      <c r="E6" s="237"/>
-      <c r="F6" s="237"/>
-      <c r="G6" s="237"/>
-      <c r="H6" s="237"/>
-      <c r="I6" s="237"/>
-      <c r="J6" s="237"/>
-      <c r="K6" s="237"/>
-      <c r="L6" s="237"/>
-      <c r="M6" s="237"/>
-      <c r="N6" s="237"/>
-      <c r="O6" s="237"/>
-      <c r="P6" s="237"/>
-      <c r="Q6" s="237"/>
-      <c r="R6" s="237"/>
-      <c r="S6" s="237"/>
-      <c r="T6" s="237"/>
-      <c r="U6" s="237"/>
-      <c r="V6" s="237"/>
-      <c r="W6" s="237"/>
-      <c r="X6" s="237"/>
-      <c r="Y6" s="237"/>
-      <c r="Z6" s="237"/>
-      <c r="AA6" s="237"/>
-      <c r="AB6" s="237"/>
-      <c r="AC6" s="237"/>
-      <c r="AD6" s="237"/>
-      <c r="AE6" s="237"/>
-      <c r="AF6" s="237"/>
-      <c r="AG6" s="240">
+      <c r="C6" s="238"/>
+      <c r="D6" s="238"/>
+      <c r="E6" s="238"/>
+      <c r="F6" s="238"/>
+      <c r="G6" s="238"/>
+      <c r="H6" s="238"/>
+      <c r="I6" s="238"/>
+      <c r="J6" s="238"/>
+      <c r="K6" s="238"/>
+      <c r="L6" s="238"/>
+      <c r="M6" s="238"/>
+      <c r="N6" s="238"/>
+      <c r="O6" s="238"/>
+      <c r="P6" s="238"/>
+      <c r="Q6" s="238"/>
+      <c r="R6" s="238"/>
+      <c r="S6" s="238"/>
+      <c r="T6" s="238"/>
+      <c r="U6" s="238"/>
+      <c r="V6" s="238"/>
+      <c r="W6" s="238"/>
+      <c r="X6" s="238"/>
+      <c r="Y6" s="238"/>
+      <c r="Z6" s="238"/>
+      <c r="AA6" s="238"/>
+      <c r="AB6" s="238"/>
+      <c r="AC6" s="238"/>
+      <c r="AD6" s="238"/>
+      <c r="AE6" s="238"/>
+      <c r="AF6" s="238"/>
+      <c r="AG6" s="241">
         <v>2</v>
       </c>
-      <c r="AH6" s="237"/>
-      <c r="AI6" s="237"/>
-      <c r="AJ6" s="237"/>
-      <c r="AK6" s="237"/>
-      <c r="AL6" s="237"/>
-      <c r="AM6" s="237"/>
-      <c r="AN6" s="237"/>
-      <c r="AO6" s="237"/>
-      <c r="AP6" s="237"/>
-      <c r="AQ6" s="237"/>
-      <c r="AR6" s="237"/>
-      <c r="AS6" s="237"/>
-      <c r="AT6" s="237"/>
-      <c r="AU6" s="237"/>
-      <c r="AV6" s="237"/>
-      <c r="AW6" s="237"/>
-      <c r="AX6" s="237"/>
-      <c r="AY6" s="237"/>
-      <c r="AZ6" s="237"/>
-      <c r="BA6" s="237"/>
-      <c r="BB6" s="237"/>
-      <c r="BC6" s="237"/>
-      <c r="BD6" s="237"/>
-      <c r="BE6" s="237"/>
-      <c r="BF6" s="237"/>
-      <c r="BG6" s="237"/>
-      <c r="BH6" s="238"/>
-      <c r="BI6" s="237">
+      <c r="AH6" s="238"/>
+      <c r="AI6" s="238"/>
+      <c r="AJ6" s="238"/>
+      <c r="AK6" s="238"/>
+      <c r="AL6" s="238"/>
+      <c r="AM6" s="238"/>
+      <c r="AN6" s="238"/>
+      <c r="AO6" s="238"/>
+      <c r="AP6" s="238"/>
+      <c r="AQ6" s="238"/>
+      <c r="AR6" s="238"/>
+      <c r="AS6" s="238"/>
+      <c r="AT6" s="238"/>
+      <c r="AU6" s="238"/>
+      <c r="AV6" s="238"/>
+      <c r="AW6" s="238"/>
+      <c r="AX6" s="238"/>
+      <c r="AY6" s="238"/>
+      <c r="AZ6" s="238"/>
+      <c r="BA6" s="238"/>
+      <c r="BB6" s="238"/>
+      <c r="BC6" s="238"/>
+      <c r="BD6" s="238"/>
+      <c r="BE6" s="238"/>
+      <c r="BF6" s="238"/>
+      <c r="BG6" s="238"/>
+      <c r="BH6" s="239"/>
+      <c r="BI6" s="238">
         <v>3</v>
       </c>
-      <c r="BJ6" s="237"/>
-      <c r="BK6" s="237"/>
-      <c r="BL6" s="237"/>
-      <c r="BM6" s="237"/>
-      <c r="BN6" s="237"/>
-      <c r="BO6" s="237"/>
-      <c r="BP6" s="237"/>
-      <c r="BQ6" s="237"/>
-      <c r="BR6" s="237"/>
-      <c r="BS6" s="237"/>
-      <c r="BT6" s="237"/>
-      <c r="BU6" s="237"/>
-      <c r="BV6" s="237"/>
-      <c r="BW6" s="237"/>
-      <c r="BX6" s="237"/>
-      <c r="BY6" s="237"/>
-      <c r="BZ6" s="237"/>
-      <c r="CA6" s="237"/>
-      <c r="CB6" s="237"/>
-      <c r="CC6" s="237"/>
-      <c r="CD6" s="237"/>
-      <c r="CE6" s="237"/>
-      <c r="CF6" s="237"/>
-      <c r="CG6" s="237"/>
-      <c r="CH6" s="237"/>
-      <c r="CI6" s="237"/>
-      <c r="CJ6" s="237"/>
-      <c r="CK6" s="237"/>
-      <c r="CL6" s="237"/>
-      <c r="CM6" s="237"/>
-      <c r="CN6" s="241">
+      <c r="BJ6" s="238"/>
+      <c r="BK6" s="238"/>
+      <c r="BL6" s="238"/>
+      <c r="BM6" s="238"/>
+      <c r="BN6" s="238"/>
+      <c r="BO6" s="238"/>
+      <c r="BP6" s="238"/>
+      <c r="BQ6" s="238"/>
+      <c r="BR6" s="238"/>
+      <c r="BS6" s="238"/>
+      <c r="BT6" s="238"/>
+      <c r="BU6" s="238"/>
+      <c r="BV6" s="238"/>
+      <c r="BW6" s="238"/>
+      <c r="BX6" s="238"/>
+      <c r="BY6" s="238"/>
+      <c r="BZ6" s="238"/>
+      <c r="CA6" s="238"/>
+      <c r="CB6" s="238"/>
+      <c r="CC6" s="238"/>
+      <c r="CD6" s="238"/>
+      <c r="CE6" s="238"/>
+      <c r="CF6" s="238"/>
+      <c r="CG6" s="238"/>
+      <c r="CH6" s="238"/>
+      <c r="CI6" s="238"/>
+      <c r="CJ6" s="238"/>
+      <c r="CK6" s="238"/>
+      <c r="CL6" s="238"/>
+      <c r="CM6" s="238"/>
+      <c r="CN6" s="242">
         <v>4</v>
       </c>
-      <c r="CO6" s="242"/>
-      <c r="CP6" s="242"/>
-      <c r="CQ6" s="242"/>
-      <c r="CR6" s="242"/>
-      <c r="CS6" s="242"/>
-      <c r="CT6" s="242"/>
-      <c r="CU6" s="242"/>
-      <c r="CV6" s="242"/>
-      <c r="CW6" s="242"/>
-      <c r="CX6" s="242"/>
-      <c r="CY6" s="242"/>
-      <c r="CZ6" s="242"/>
-      <c r="DA6" s="242"/>
-      <c r="DB6" s="242"/>
-      <c r="DC6" s="242"/>
-      <c r="DD6" s="242"/>
-      <c r="DE6" s="242"/>
-      <c r="DF6" s="242"/>
-      <c r="DG6" s="242"/>
-      <c r="DH6" s="242"/>
-      <c r="DI6" s="242"/>
-      <c r="DJ6" s="242"/>
-      <c r="DK6" s="242"/>
-      <c r="DL6" s="242"/>
-      <c r="DM6" s="242"/>
-      <c r="DN6" s="242"/>
-      <c r="DO6" s="242"/>
-      <c r="DP6" s="242"/>
-      <c r="DQ6" s="243"/>
-      <c r="DR6" s="237">
+      <c r="CO6" s="243"/>
+      <c r="CP6" s="243"/>
+      <c r="CQ6" s="243"/>
+      <c r="CR6" s="243"/>
+      <c r="CS6" s="243"/>
+      <c r="CT6" s="243"/>
+      <c r="CU6" s="243"/>
+      <c r="CV6" s="243"/>
+      <c r="CW6" s="243"/>
+      <c r="CX6" s="243"/>
+      <c r="CY6" s="243"/>
+      <c r="CZ6" s="243"/>
+      <c r="DA6" s="243"/>
+      <c r="DB6" s="243"/>
+      <c r="DC6" s="243"/>
+      <c r="DD6" s="243"/>
+      <c r="DE6" s="243"/>
+      <c r="DF6" s="243"/>
+      <c r="DG6" s="243"/>
+      <c r="DH6" s="243"/>
+      <c r="DI6" s="243"/>
+      <c r="DJ6" s="243"/>
+      <c r="DK6" s="243"/>
+      <c r="DL6" s="243"/>
+      <c r="DM6" s="243"/>
+      <c r="DN6" s="243"/>
+      <c r="DO6" s="243"/>
+      <c r="DP6" s="243"/>
+      <c r="DQ6" s="244"/>
+      <c r="DR6" s="238">
         <v>5</v>
       </c>
-      <c r="DS6" s="237"/>
-      <c r="DT6" s="237"/>
-      <c r="DU6" s="237"/>
-      <c r="DV6" s="237"/>
-      <c r="DW6" s="237"/>
-      <c r="DX6" s="237"/>
-      <c r="DY6" s="237"/>
-      <c r="DZ6" s="237"/>
-      <c r="EA6" s="237"/>
-      <c r="EB6" s="237"/>
-      <c r="EC6" s="237"/>
-      <c r="ED6" s="237"/>
-      <c r="EE6" s="237"/>
-      <c r="EF6" s="237"/>
-      <c r="EG6" s="237"/>
-      <c r="EH6" s="237"/>
-      <c r="EI6" s="237"/>
-      <c r="EJ6" s="237"/>
-      <c r="EK6" s="237"/>
-      <c r="EL6" s="237"/>
-      <c r="EM6" s="237"/>
-      <c r="EN6" s="237"/>
-      <c r="EO6" s="237"/>
-      <c r="EP6" s="237"/>
-      <c r="EQ6" s="237"/>
-      <c r="ER6" s="237"/>
-      <c r="ES6" s="237"/>
-      <c r="ET6" s="237"/>
-      <c r="EU6" s="237"/>
-      <c r="EV6" s="238"/>
-      <c r="EW6" s="241">
+      <c r="DS6" s="238"/>
+      <c r="DT6" s="238"/>
+      <c r="DU6" s="238"/>
+      <c r="DV6" s="238"/>
+      <c r="DW6" s="238"/>
+      <c r="DX6" s="238"/>
+      <c r="DY6" s="238"/>
+      <c r="DZ6" s="238"/>
+      <c r="EA6" s="238"/>
+      <c r="EB6" s="238"/>
+      <c r="EC6" s="238"/>
+      <c r="ED6" s="238"/>
+      <c r="EE6" s="238"/>
+      <c r="EF6" s="238"/>
+      <c r="EG6" s="238"/>
+      <c r="EH6" s="238"/>
+      <c r="EI6" s="238"/>
+      <c r="EJ6" s="238"/>
+      <c r="EK6" s="238"/>
+      <c r="EL6" s="238"/>
+      <c r="EM6" s="238"/>
+      <c r="EN6" s="238"/>
+      <c r="EO6" s="238"/>
+      <c r="EP6" s="238"/>
+      <c r="EQ6" s="238"/>
+      <c r="ER6" s="238"/>
+      <c r="ES6" s="238"/>
+      <c r="ET6" s="238"/>
+      <c r="EU6" s="238"/>
+      <c r="EV6" s="239"/>
+      <c r="EW6" s="242">
         <v>6</v>
       </c>
-      <c r="EX6" s="242"/>
-      <c r="EY6" s="242"/>
-      <c r="EZ6" s="242"/>
-      <c r="FA6" s="242"/>
-      <c r="FB6" s="242"/>
-      <c r="FC6" s="242"/>
-      <c r="FD6" s="242"/>
-      <c r="FE6" s="242"/>
-      <c r="FF6" s="242"/>
-      <c r="FG6" s="242"/>
-      <c r="FH6" s="242"/>
-      <c r="FI6" s="242"/>
-      <c r="FJ6" s="242"/>
-      <c r="FK6" s="242"/>
-      <c r="FL6" s="242"/>
-      <c r="FM6" s="242"/>
-      <c r="FN6" s="242"/>
-      <c r="FO6" s="242"/>
-      <c r="FP6" s="242"/>
-      <c r="FQ6" s="242"/>
-      <c r="FR6" s="242"/>
-      <c r="FS6" s="242"/>
-      <c r="FT6" s="242"/>
-      <c r="FU6" s="242"/>
-      <c r="FV6" s="242"/>
-      <c r="FW6" s="242"/>
-      <c r="FX6" s="242"/>
-      <c r="FY6" s="242"/>
-      <c r="FZ6" s="243"/>
-      <c r="GA6" s="237">
+      <c r="EX6" s="243"/>
+      <c r="EY6" s="243"/>
+      <c r="EZ6" s="243"/>
+      <c r="FA6" s="243"/>
+      <c r="FB6" s="243"/>
+      <c r="FC6" s="243"/>
+      <c r="FD6" s="243"/>
+      <c r="FE6" s="243"/>
+      <c r="FF6" s="243"/>
+      <c r="FG6" s="243"/>
+      <c r="FH6" s="243"/>
+      <c r="FI6" s="243"/>
+      <c r="FJ6" s="243"/>
+      <c r="FK6" s="243"/>
+      <c r="FL6" s="243"/>
+      <c r="FM6" s="243"/>
+      <c r="FN6" s="243"/>
+      <c r="FO6" s="243"/>
+      <c r="FP6" s="243"/>
+      <c r="FQ6" s="243"/>
+      <c r="FR6" s="243"/>
+      <c r="FS6" s="243"/>
+      <c r="FT6" s="243"/>
+      <c r="FU6" s="243"/>
+      <c r="FV6" s="243"/>
+      <c r="FW6" s="243"/>
+      <c r="FX6" s="243"/>
+      <c r="FY6" s="243"/>
+      <c r="FZ6" s="244"/>
+      <c r="GA6" s="238">
         <v>7</v>
       </c>
-      <c r="GB6" s="237"/>
-      <c r="GC6" s="237"/>
-      <c r="GD6" s="237"/>
-      <c r="GE6" s="237"/>
-      <c r="GF6" s="237"/>
-      <c r="GG6" s="237"/>
-      <c r="GH6" s="237"/>
-      <c r="GI6" s="237"/>
-      <c r="GJ6" s="237"/>
-      <c r="GK6" s="237"/>
-      <c r="GL6" s="237"/>
-      <c r="GM6" s="237"/>
-      <c r="GN6" s="237"/>
-      <c r="GO6" s="237"/>
-      <c r="GP6" s="237"/>
-      <c r="GQ6" s="237"/>
-      <c r="GR6" s="237"/>
-      <c r="GS6" s="237"/>
-      <c r="GT6" s="237"/>
-      <c r="GU6" s="237"/>
-      <c r="GV6" s="237"/>
-      <c r="GW6" s="237"/>
-      <c r="GX6" s="237"/>
-      <c r="GY6" s="237"/>
-      <c r="GZ6" s="237"/>
-      <c r="HA6" s="237"/>
-      <c r="HB6" s="237"/>
-      <c r="HC6" s="237"/>
-      <c r="HD6" s="237"/>
-      <c r="HE6" s="238"/>
-      <c r="HF6" s="237">
+      <c r="GB6" s="238"/>
+      <c r="GC6" s="238"/>
+      <c r="GD6" s="238"/>
+      <c r="GE6" s="238"/>
+      <c r="GF6" s="238"/>
+      <c r="GG6" s="238"/>
+      <c r="GH6" s="238"/>
+      <c r="GI6" s="238"/>
+      <c r="GJ6" s="238"/>
+      <c r="GK6" s="238"/>
+      <c r="GL6" s="238"/>
+      <c r="GM6" s="238"/>
+      <c r="GN6" s="238"/>
+      <c r="GO6" s="238"/>
+      <c r="GP6" s="238"/>
+      <c r="GQ6" s="238"/>
+      <c r="GR6" s="238"/>
+      <c r="GS6" s="238"/>
+      <c r="GT6" s="238"/>
+      <c r="GU6" s="238"/>
+      <c r="GV6" s="238"/>
+      <c r="GW6" s="238"/>
+      <c r="GX6" s="238"/>
+      <c r="GY6" s="238"/>
+      <c r="GZ6" s="238"/>
+      <c r="HA6" s="238"/>
+      <c r="HB6" s="238"/>
+      <c r="HC6" s="238"/>
+      <c r="HD6" s="238"/>
+      <c r="HE6" s="239"/>
+      <c r="HF6" s="238">
         <v>8</v>
       </c>
-      <c r="HG6" s="237"/>
-      <c r="HH6" s="237"/>
-      <c r="HI6" s="237"/>
-      <c r="HJ6" s="237"/>
-      <c r="HK6" s="237"/>
-      <c r="HL6" s="237"/>
-      <c r="HM6" s="237"/>
-      <c r="HN6" s="237"/>
-      <c r="HO6" s="237"/>
-      <c r="HP6" s="237"/>
-      <c r="HQ6" s="237"/>
-      <c r="HR6" s="237"/>
-      <c r="HS6" s="237"/>
-      <c r="HT6" s="237"/>
-      <c r="HU6" s="237"/>
-      <c r="HV6" s="237"/>
-      <c r="HW6" s="237"/>
-      <c r="HX6" s="237"/>
-      <c r="HY6" s="237"/>
-      <c r="HZ6" s="237"/>
-      <c r="IA6" s="237"/>
-      <c r="IB6" s="237"/>
-      <c r="IC6" s="237"/>
-      <c r="ID6" s="237"/>
-      <c r="IE6" s="237"/>
-      <c r="IF6" s="237"/>
-      <c r="IG6" s="237"/>
-      <c r="IH6" s="237"/>
-      <c r="II6" s="237"/>
-      <c r="IJ6" s="238"/>
-      <c r="IK6" s="241">
+      <c r="HG6" s="238"/>
+      <c r="HH6" s="238"/>
+      <c r="HI6" s="238"/>
+      <c r="HJ6" s="238"/>
+      <c r="HK6" s="238"/>
+      <c r="HL6" s="238"/>
+      <c r="HM6" s="238"/>
+      <c r="HN6" s="238"/>
+      <c r="HO6" s="238"/>
+      <c r="HP6" s="238"/>
+      <c r="HQ6" s="238"/>
+      <c r="HR6" s="238"/>
+      <c r="HS6" s="238"/>
+      <c r="HT6" s="238"/>
+      <c r="HU6" s="238"/>
+      <c r="HV6" s="238"/>
+      <c r="HW6" s="238"/>
+      <c r="HX6" s="238"/>
+      <c r="HY6" s="238"/>
+      <c r="HZ6" s="238"/>
+      <c r="IA6" s="238"/>
+      <c r="IB6" s="238"/>
+      <c r="IC6" s="238"/>
+      <c r="ID6" s="238"/>
+      <c r="IE6" s="238"/>
+      <c r="IF6" s="238"/>
+      <c r="IG6" s="238"/>
+      <c r="IH6" s="238"/>
+      <c r="II6" s="238"/>
+      <c r="IJ6" s="239"/>
+      <c r="IK6" s="242">
         <v>9</v>
       </c>
-      <c r="IL6" s="242"/>
-      <c r="IM6" s="242"/>
-      <c r="IN6" s="242"/>
-      <c r="IO6" s="242"/>
-      <c r="IP6" s="242"/>
-      <c r="IQ6" s="242"/>
-      <c r="IR6" s="242"/>
-      <c r="IS6" s="242"/>
-      <c r="IT6" s="242"/>
-      <c r="IU6" s="242"/>
-      <c r="IV6" s="242"/>
-      <c r="IW6" s="242"/>
-      <c r="IX6" s="242"/>
-      <c r="IY6" s="242"/>
-      <c r="IZ6" s="242"/>
-      <c r="JA6" s="242"/>
-      <c r="JB6" s="242"/>
-      <c r="JC6" s="242"/>
-      <c r="JD6" s="242"/>
-      <c r="JE6" s="242"/>
-      <c r="JF6" s="242"/>
-      <c r="JG6" s="242"/>
-      <c r="JH6" s="242"/>
-      <c r="JI6" s="242"/>
-      <c r="JJ6" s="242"/>
-      <c r="JK6" s="242"/>
-      <c r="JL6" s="242"/>
-      <c r="JM6" s="242"/>
-      <c r="JN6" s="243"/>
-      <c r="JO6" s="237">
+      <c r="IL6" s="243"/>
+      <c r="IM6" s="243"/>
+      <c r="IN6" s="243"/>
+      <c r="IO6" s="243"/>
+      <c r="IP6" s="243"/>
+      <c r="IQ6" s="243"/>
+      <c r="IR6" s="243"/>
+      <c r="IS6" s="243"/>
+      <c r="IT6" s="243"/>
+      <c r="IU6" s="243"/>
+      <c r="IV6" s="243"/>
+      <c r="IW6" s="243"/>
+      <c r="IX6" s="243"/>
+      <c r="IY6" s="243"/>
+      <c r="IZ6" s="243"/>
+      <c r="JA6" s="243"/>
+      <c r="JB6" s="243"/>
+      <c r="JC6" s="243"/>
+      <c r="JD6" s="243"/>
+      <c r="JE6" s="243"/>
+      <c r="JF6" s="243"/>
+      <c r="JG6" s="243"/>
+      <c r="JH6" s="243"/>
+      <c r="JI6" s="243"/>
+      <c r="JJ6" s="243"/>
+      <c r="JK6" s="243"/>
+      <c r="JL6" s="243"/>
+      <c r="JM6" s="243"/>
+      <c r="JN6" s="244"/>
+      <c r="JO6" s="238">
         <v>10</v>
       </c>
-      <c r="JP6" s="237"/>
-      <c r="JQ6" s="237"/>
-      <c r="JR6" s="237"/>
-      <c r="JS6" s="237"/>
-      <c r="JT6" s="237"/>
-      <c r="JU6" s="237"/>
-      <c r="JV6" s="237"/>
-      <c r="JW6" s="237"/>
-      <c r="JX6" s="237"/>
-      <c r="JY6" s="237"/>
-      <c r="JZ6" s="237"/>
-      <c r="KA6" s="237"/>
-      <c r="KB6" s="237"/>
-      <c r="KC6" s="237"/>
-      <c r="KD6" s="237"/>
-      <c r="KE6" s="237"/>
-      <c r="KF6" s="237"/>
-      <c r="KG6" s="237"/>
-      <c r="KH6" s="237"/>
-      <c r="KI6" s="237"/>
-      <c r="KJ6" s="237"/>
-      <c r="KK6" s="237"/>
-      <c r="KL6" s="237"/>
-      <c r="KM6" s="237"/>
-      <c r="KN6" s="237"/>
-      <c r="KO6" s="237"/>
-      <c r="KP6" s="237"/>
-      <c r="KQ6" s="237"/>
-      <c r="KR6" s="237"/>
-      <c r="KS6" s="238"/>
-      <c r="KT6" s="241">
+      <c r="JP6" s="238"/>
+      <c r="JQ6" s="238"/>
+      <c r="JR6" s="238"/>
+      <c r="JS6" s="238"/>
+      <c r="JT6" s="238"/>
+      <c r="JU6" s="238"/>
+      <c r="JV6" s="238"/>
+      <c r="JW6" s="238"/>
+      <c r="JX6" s="238"/>
+      <c r="JY6" s="238"/>
+      <c r="JZ6" s="238"/>
+      <c r="KA6" s="238"/>
+      <c r="KB6" s="238"/>
+      <c r="KC6" s="238"/>
+      <c r="KD6" s="238"/>
+      <c r="KE6" s="238"/>
+      <c r="KF6" s="238"/>
+      <c r="KG6" s="238"/>
+      <c r="KH6" s="238"/>
+      <c r="KI6" s="238"/>
+      <c r="KJ6" s="238"/>
+      <c r="KK6" s="238"/>
+      <c r="KL6" s="238"/>
+      <c r="KM6" s="238"/>
+      <c r="KN6" s="238"/>
+      <c r="KO6" s="238"/>
+      <c r="KP6" s="238"/>
+      <c r="KQ6" s="238"/>
+      <c r="KR6" s="238"/>
+      <c r="KS6" s="239"/>
+      <c r="KT6" s="242">
         <v>11</v>
       </c>
-      <c r="KU6" s="242"/>
-      <c r="KV6" s="242"/>
-      <c r="KW6" s="242"/>
-      <c r="KX6" s="242"/>
-      <c r="KY6" s="242"/>
-      <c r="KZ6" s="242"/>
-      <c r="LA6" s="242"/>
-      <c r="LB6" s="242"/>
-      <c r="LC6" s="242"/>
-      <c r="LD6" s="242"/>
-      <c r="LE6" s="242"/>
-      <c r="LF6" s="242"/>
-      <c r="LG6" s="242"/>
-      <c r="LH6" s="242"/>
-      <c r="LI6" s="242"/>
-      <c r="LJ6" s="242"/>
-      <c r="LK6" s="242"/>
-      <c r="LL6" s="242"/>
-      <c r="LM6" s="242"/>
-      <c r="LN6" s="242"/>
-      <c r="LO6" s="242"/>
-      <c r="LP6" s="242"/>
-      <c r="LQ6" s="242"/>
-      <c r="LR6" s="242"/>
-      <c r="LS6" s="242"/>
-      <c r="LT6" s="242"/>
-      <c r="LU6" s="242"/>
-      <c r="LV6" s="242"/>
-      <c r="LW6" s="243"/>
-      <c r="LX6" s="237">
+      <c r="KU6" s="243"/>
+      <c r="KV6" s="243"/>
+      <c r="KW6" s="243"/>
+      <c r="KX6" s="243"/>
+      <c r="KY6" s="243"/>
+      <c r="KZ6" s="243"/>
+      <c r="LA6" s="243"/>
+      <c r="LB6" s="243"/>
+      <c r="LC6" s="243"/>
+      <c r="LD6" s="243"/>
+      <c r="LE6" s="243"/>
+      <c r="LF6" s="243"/>
+      <c r="LG6" s="243"/>
+      <c r="LH6" s="243"/>
+      <c r="LI6" s="243"/>
+      <c r="LJ6" s="243"/>
+      <c r="LK6" s="243"/>
+      <c r="LL6" s="243"/>
+      <c r="LM6" s="243"/>
+      <c r="LN6" s="243"/>
+      <c r="LO6" s="243"/>
+      <c r="LP6" s="243"/>
+      <c r="LQ6" s="243"/>
+      <c r="LR6" s="243"/>
+      <c r="LS6" s="243"/>
+      <c r="LT6" s="243"/>
+      <c r="LU6" s="243"/>
+      <c r="LV6" s="243"/>
+      <c r="LW6" s="244"/>
+      <c r="LX6" s="238">
         <v>12</v>
       </c>
-      <c r="LY6" s="237"/>
-      <c r="LZ6" s="237"/>
-      <c r="MA6" s="237"/>
-      <c r="MB6" s="237"/>
-      <c r="MC6" s="237"/>
-      <c r="MD6" s="237"/>
-      <c r="ME6" s="237"/>
-      <c r="MF6" s="237"/>
-      <c r="MG6" s="237"/>
-      <c r="MH6" s="237"/>
-      <c r="MI6" s="237"/>
-      <c r="MJ6" s="237"/>
-      <c r="MK6" s="237"/>
-      <c r="ML6" s="237"/>
-      <c r="MM6" s="237"/>
-      <c r="MN6" s="237"/>
-      <c r="MO6" s="237"/>
-      <c r="MP6" s="237"/>
-      <c r="MQ6" s="237"/>
-      <c r="MR6" s="237"/>
-      <c r="MS6" s="237"/>
-      <c r="MT6" s="237"/>
-      <c r="MU6" s="237"/>
-      <c r="MV6" s="237"/>
-      <c r="MW6" s="237"/>
-      <c r="MX6" s="237"/>
-      <c r="MY6" s="237"/>
-      <c r="MZ6" s="237"/>
-      <c r="NA6" s="237"/>
-      <c r="NB6" s="238"/>
+      <c r="LY6" s="238"/>
+      <c r="LZ6" s="238"/>
+      <c r="MA6" s="238"/>
+      <c r="MB6" s="238"/>
+      <c r="MC6" s="238"/>
+      <c r="MD6" s="238"/>
+      <c r="ME6" s="238"/>
+      <c r="MF6" s="238"/>
+      <c r="MG6" s="238"/>
+      <c r="MH6" s="238"/>
+      <c r="MI6" s="238"/>
+      <c r="MJ6" s="238"/>
+      <c r="MK6" s="238"/>
+      <c r="ML6" s="238"/>
+      <c r="MM6" s="238"/>
+      <c r="MN6" s="238"/>
+      <c r="MO6" s="238"/>
+      <c r="MP6" s="238"/>
+      <c r="MQ6" s="238"/>
+      <c r="MR6" s="238"/>
+      <c r="MS6" s="238"/>
+      <c r="MT6" s="238"/>
+      <c r="MU6" s="238"/>
+      <c r="MV6" s="238"/>
+      <c r="MW6" s="238"/>
+      <c r="MX6" s="238"/>
+      <c r="MY6" s="238"/>
+      <c r="MZ6" s="238"/>
+      <c r="NA6" s="238"/>
+      <c r="NB6" s="239"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -18188,7 +18192,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="244" t="s">
+      <c r="A8" s="245" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -18576,7 +18580,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="244"/>
+      <c r="A9" s="245"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -18956,7 +18960,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="244"/>
+      <c r="A10" s="245"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -19336,7 +19340,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="244"/>
+      <c r="A11" s="245"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -19712,7 +19716,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="244"/>
+      <c r="A12" s="245"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -20086,7 +20090,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="244"/>
+      <c r="A13" s="245"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -20456,7 +20460,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="244"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -20826,7 +20830,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="244" t="s">
+      <c r="A15" s="245" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -21210,7 +21214,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="244"/>
+      <c r="A16" s="245"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -21590,7 +21594,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="244"/>
+      <c r="A17" s="245"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -21966,7 +21970,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="244"/>
+      <c r="A18" s="245"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -22342,7 +22346,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="244"/>
+      <c r="A19" s="245"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -22712,7 +22716,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="244" t="s">
+      <c r="A20" s="245" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -23090,7 +23094,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="244"/>
+      <c r="A21" s="245"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -23464,7 +23468,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="244"/>
+      <c r="A22" s="245"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -23836,7 +23840,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="244"/>
+      <c r="A23" s="245"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -24212,7 +24216,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="244"/>
+      <c r="A24" s="245"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -24580,7 +24584,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="245" t="s">
+      <c r="A25" s="246" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="75"/>
@@ -24956,7 +24960,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="244"/>
+      <c r="A26" s="245"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -25328,7 +25332,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="244"/>
+      <c r="A27" s="245"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -25702,7 +25706,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="244"/>
+      <c r="A28" s="245"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -26074,7 +26078,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="244"/>
+      <c r="A29" s="245"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -26444,7 +26448,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="245" t="s">
+      <c r="A30" s="246" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -26816,7 +26820,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="244"/>
+      <c r="A31" s="245"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -27190,7 +27194,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="244"/>
+      <c r="A32" s="245"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -27564,7 +27568,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="244"/>
+      <c r="A33" s="245"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -27934,7 +27938,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="244"/>
+      <c r="A34" s="245"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -28302,7 +28306,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="244" t="s">
+      <c r="A35" s="245" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -28684,7 +28688,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="244"/>
+      <c r="A36" s="245"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -29056,7 +29060,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="244"/>
+      <c r="A37" s="245"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -29434,7 +29438,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="244"/>
+      <c r="A38" s="245"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -29804,7 +29808,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="244"/>
+      <c r="A39" s="245"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -30176,7 +30180,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="244" t="s">
+      <c r="A40" s="245" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -30554,7 +30558,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="244"/>
+      <c r="A41" s="245"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -30928,7 +30932,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="244"/>
+      <c r="A42" s="245"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -31300,7 +31304,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="244"/>
+      <c r="A43" s="245"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -31670,7 +31674,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="244"/>
+      <c r="A44" s="245"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -32038,7 +32042,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="244" t="s">
+      <c r="A45" s="245" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -32418,7 +32422,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="244"/>
+      <c r="A46" s="245"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -32788,7 +32792,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="244"/>
+      <c r="A47" s="245"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -33164,7 +33168,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="244"/>
+      <c r="A48" s="245"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -33534,7 +33538,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="244"/>
+      <c r="A49" s="245"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -33908,7 +33912,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="244" t="s">
+      <c r="A50" s="245" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -34290,7 +34294,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="244"/>
+      <c r="A51" s="245"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -34668,7 +34672,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="244"/>
+      <c r="A52" s="245"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -35040,7 +35044,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="244"/>
+      <c r="A53" s="245"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -35410,7 +35414,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="244"/>
+      <c r="A54" s="245"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -35796,6 +35800,11 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="GA6:HE6"/>
+    <mergeCell ref="HF6:IJ6"/>
+    <mergeCell ref="IK6:JN6"/>
+    <mergeCell ref="JO6:KS6"/>
+    <mergeCell ref="KT6:LW6"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A15:A19"/>
@@ -35812,11 +35821,6 @@
     <mergeCell ref="BI6:CM6"/>
     <mergeCell ref="CN6:DQ6"/>
     <mergeCell ref="DR6:EV6"/>
-    <mergeCell ref="GA6:HE6"/>
-    <mergeCell ref="HF6:IJ6"/>
-    <mergeCell ref="IK6:JN6"/>
-    <mergeCell ref="JO6:KS6"/>
-    <mergeCell ref="KT6:LW6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35869,395 +35873,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="240">
+      <c r="B6" s="241">
         <v>1</v>
       </c>
-      <c r="C6" s="237"/>
-      <c r="D6" s="237"/>
-      <c r="E6" s="237"/>
-      <c r="F6" s="237"/>
-      <c r="G6" s="237"/>
-      <c r="H6" s="237"/>
-      <c r="I6" s="237"/>
-      <c r="J6" s="237"/>
-      <c r="K6" s="237"/>
-      <c r="L6" s="237"/>
-      <c r="M6" s="237"/>
-      <c r="N6" s="237"/>
-      <c r="O6" s="237"/>
-      <c r="P6" s="237"/>
-      <c r="Q6" s="237"/>
-      <c r="R6" s="237"/>
-      <c r="S6" s="237"/>
-      <c r="T6" s="237"/>
-      <c r="U6" s="237"/>
-      <c r="V6" s="237"/>
-      <c r="W6" s="237"/>
-      <c r="X6" s="237"/>
-      <c r="Y6" s="237"/>
-      <c r="Z6" s="237"/>
-      <c r="AA6" s="237"/>
-      <c r="AB6" s="237"/>
-      <c r="AC6" s="237"/>
-      <c r="AD6" s="237"/>
-      <c r="AE6" s="237"/>
-      <c r="AF6" s="237"/>
-      <c r="AG6" s="240">
+      <c r="C6" s="238"/>
+      <c r="D6" s="238"/>
+      <c r="E6" s="238"/>
+      <c r="F6" s="238"/>
+      <c r="G6" s="238"/>
+      <c r="H6" s="238"/>
+      <c r="I6" s="238"/>
+      <c r="J6" s="238"/>
+      <c r="K6" s="238"/>
+      <c r="L6" s="238"/>
+      <c r="M6" s="238"/>
+      <c r="N6" s="238"/>
+      <c r="O6" s="238"/>
+      <c r="P6" s="238"/>
+      <c r="Q6" s="238"/>
+      <c r="R6" s="238"/>
+      <c r="S6" s="238"/>
+      <c r="T6" s="238"/>
+      <c r="U6" s="238"/>
+      <c r="V6" s="238"/>
+      <c r="W6" s="238"/>
+      <c r="X6" s="238"/>
+      <c r="Y6" s="238"/>
+      <c r="Z6" s="238"/>
+      <c r="AA6" s="238"/>
+      <c r="AB6" s="238"/>
+      <c r="AC6" s="238"/>
+      <c r="AD6" s="238"/>
+      <c r="AE6" s="238"/>
+      <c r="AF6" s="238"/>
+      <c r="AG6" s="241">
         <v>2</v>
       </c>
-      <c r="AH6" s="237"/>
-      <c r="AI6" s="237"/>
-      <c r="AJ6" s="237"/>
-      <c r="AK6" s="237"/>
-      <c r="AL6" s="237"/>
-      <c r="AM6" s="237"/>
-      <c r="AN6" s="237"/>
-      <c r="AO6" s="237"/>
-      <c r="AP6" s="237"/>
-      <c r="AQ6" s="237"/>
-      <c r="AR6" s="237"/>
-      <c r="AS6" s="237"/>
-      <c r="AT6" s="237"/>
-      <c r="AU6" s="237"/>
-      <c r="AV6" s="237"/>
-      <c r="AW6" s="237"/>
-      <c r="AX6" s="237"/>
-      <c r="AY6" s="237"/>
-      <c r="AZ6" s="237"/>
-      <c r="BA6" s="237"/>
-      <c r="BB6" s="237"/>
-      <c r="BC6" s="237"/>
-      <c r="BD6" s="237"/>
-      <c r="BE6" s="237"/>
-      <c r="BF6" s="237"/>
-      <c r="BG6" s="237"/>
-      <c r="BH6" s="238"/>
-      <c r="BI6" s="237">
+      <c r="AH6" s="238"/>
+      <c r="AI6" s="238"/>
+      <c r="AJ6" s="238"/>
+      <c r="AK6" s="238"/>
+      <c r="AL6" s="238"/>
+      <c r="AM6" s="238"/>
+      <c r="AN6" s="238"/>
+      <c r="AO6" s="238"/>
+      <c r="AP6" s="238"/>
+      <c r="AQ6" s="238"/>
+      <c r="AR6" s="238"/>
+      <c r="AS6" s="238"/>
+      <c r="AT6" s="238"/>
+      <c r="AU6" s="238"/>
+      <c r="AV6" s="238"/>
+      <c r="AW6" s="238"/>
+      <c r="AX6" s="238"/>
+      <c r="AY6" s="238"/>
+      <c r="AZ6" s="238"/>
+      <c r="BA6" s="238"/>
+      <c r="BB6" s="238"/>
+      <c r="BC6" s="238"/>
+      <c r="BD6" s="238"/>
+      <c r="BE6" s="238"/>
+      <c r="BF6" s="238"/>
+      <c r="BG6" s="238"/>
+      <c r="BH6" s="239"/>
+      <c r="BI6" s="238">
         <v>3</v>
       </c>
-      <c r="BJ6" s="237"/>
-      <c r="BK6" s="237"/>
-      <c r="BL6" s="237"/>
-      <c r="BM6" s="237"/>
-      <c r="BN6" s="237"/>
-      <c r="BO6" s="237"/>
-      <c r="BP6" s="237"/>
-      <c r="BQ6" s="237"/>
-      <c r="BR6" s="237"/>
-      <c r="BS6" s="237"/>
-      <c r="BT6" s="237"/>
-      <c r="BU6" s="237"/>
-      <c r="BV6" s="237"/>
-      <c r="BW6" s="237"/>
-      <c r="BX6" s="237"/>
-      <c r="BY6" s="237"/>
-      <c r="BZ6" s="237"/>
-      <c r="CA6" s="237"/>
-      <c r="CB6" s="237"/>
-      <c r="CC6" s="237"/>
-      <c r="CD6" s="237"/>
-      <c r="CE6" s="237"/>
-      <c r="CF6" s="237"/>
-      <c r="CG6" s="237"/>
-      <c r="CH6" s="237"/>
-      <c r="CI6" s="237"/>
-      <c r="CJ6" s="237"/>
-      <c r="CK6" s="237"/>
-      <c r="CL6" s="237"/>
-      <c r="CM6" s="237"/>
-      <c r="CN6" s="241">
+      <c r="BJ6" s="238"/>
+      <c r="BK6" s="238"/>
+      <c r="BL6" s="238"/>
+      <c r="BM6" s="238"/>
+      <c r="BN6" s="238"/>
+      <c r="BO6" s="238"/>
+      <c r="BP6" s="238"/>
+      <c r="BQ6" s="238"/>
+      <c r="BR6" s="238"/>
+      <c r="BS6" s="238"/>
+      <c r="BT6" s="238"/>
+      <c r="BU6" s="238"/>
+      <c r="BV6" s="238"/>
+      <c r="BW6" s="238"/>
+      <c r="BX6" s="238"/>
+      <c r="BY6" s="238"/>
+      <c r="BZ6" s="238"/>
+      <c r="CA6" s="238"/>
+      <c r="CB6" s="238"/>
+      <c r="CC6" s="238"/>
+      <c r="CD6" s="238"/>
+      <c r="CE6" s="238"/>
+      <c r="CF6" s="238"/>
+      <c r="CG6" s="238"/>
+      <c r="CH6" s="238"/>
+      <c r="CI6" s="238"/>
+      <c r="CJ6" s="238"/>
+      <c r="CK6" s="238"/>
+      <c r="CL6" s="238"/>
+      <c r="CM6" s="238"/>
+      <c r="CN6" s="242">
         <v>4</v>
       </c>
-      <c r="CO6" s="242"/>
-      <c r="CP6" s="242"/>
-      <c r="CQ6" s="242"/>
-      <c r="CR6" s="242"/>
-      <c r="CS6" s="242"/>
-      <c r="CT6" s="242"/>
-      <c r="CU6" s="242"/>
-      <c r="CV6" s="242"/>
-      <c r="CW6" s="242"/>
-      <c r="CX6" s="242"/>
-      <c r="CY6" s="242"/>
-      <c r="CZ6" s="242"/>
-      <c r="DA6" s="242"/>
-      <c r="DB6" s="242"/>
-      <c r="DC6" s="242"/>
-      <c r="DD6" s="242"/>
-      <c r="DE6" s="242"/>
-      <c r="DF6" s="242"/>
-      <c r="DG6" s="242"/>
-      <c r="DH6" s="242"/>
-      <c r="DI6" s="242"/>
-      <c r="DJ6" s="242"/>
-      <c r="DK6" s="242"/>
-      <c r="DL6" s="242"/>
-      <c r="DM6" s="242"/>
-      <c r="DN6" s="242"/>
-      <c r="DO6" s="242"/>
-      <c r="DP6" s="242"/>
-      <c r="DQ6" s="243"/>
-      <c r="DR6" s="237">
+      <c r="CO6" s="243"/>
+      <c r="CP6" s="243"/>
+      <c r="CQ6" s="243"/>
+      <c r="CR6" s="243"/>
+      <c r="CS6" s="243"/>
+      <c r="CT6" s="243"/>
+      <c r="CU6" s="243"/>
+      <c r="CV6" s="243"/>
+      <c r="CW6" s="243"/>
+      <c r="CX6" s="243"/>
+      <c r="CY6" s="243"/>
+      <c r="CZ6" s="243"/>
+      <c r="DA6" s="243"/>
+      <c r="DB6" s="243"/>
+      <c r="DC6" s="243"/>
+      <c r="DD6" s="243"/>
+      <c r="DE6" s="243"/>
+      <c r="DF6" s="243"/>
+      <c r="DG6" s="243"/>
+      <c r="DH6" s="243"/>
+      <c r="DI6" s="243"/>
+      <c r="DJ6" s="243"/>
+      <c r="DK6" s="243"/>
+      <c r="DL6" s="243"/>
+      <c r="DM6" s="243"/>
+      <c r="DN6" s="243"/>
+      <c r="DO6" s="243"/>
+      <c r="DP6" s="243"/>
+      <c r="DQ6" s="244"/>
+      <c r="DR6" s="238">
         <v>5</v>
       </c>
-      <c r="DS6" s="237"/>
-      <c r="DT6" s="237"/>
-      <c r="DU6" s="237"/>
-      <c r="DV6" s="237"/>
-      <c r="DW6" s="237"/>
-      <c r="DX6" s="237"/>
-      <c r="DY6" s="237"/>
-      <c r="DZ6" s="237"/>
-      <c r="EA6" s="237"/>
-      <c r="EB6" s="237"/>
-      <c r="EC6" s="237"/>
-      <c r="ED6" s="237"/>
-      <c r="EE6" s="237"/>
-      <c r="EF6" s="237"/>
-      <c r="EG6" s="237"/>
-      <c r="EH6" s="237"/>
-      <c r="EI6" s="237"/>
-      <c r="EJ6" s="237"/>
-      <c r="EK6" s="237"/>
-      <c r="EL6" s="237"/>
-      <c r="EM6" s="237"/>
-      <c r="EN6" s="237"/>
-      <c r="EO6" s="237"/>
-      <c r="EP6" s="237"/>
-      <c r="EQ6" s="237"/>
-      <c r="ER6" s="237"/>
-      <c r="ES6" s="237"/>
-      <c r="ET6" s="237"/>
-      <c r="EU6" s="237"/>
-      <c r="EV6" s="238"/>
-      <c r="EW6" s="241">
+      <c r="DS6" s="238"/>
+      <c r="DT6" s="238"/>
+      <c r="DU6" s="238"/>
+      <c r="DV6" s="238"/>
+      <c r="DW6" s="238"/>
+      <c r="DX6" s="238"/>
+      <c r="DY6" s="238"/>
+      <c r="DZ6" s="238"/>
+      <c r="EA6" s="238"/>
+      <c r="EB6" s="238"/>
+      <c r="EC6" s="238"/>
+      <c r="ED6" s="238"/>
+      <c r="EE6" s="238"/>
+      <c r="EF6" s="238"/>
+      <c r="EG6" s="238"/>
+      <c r="EH6" s="238"/>
+      <c r="EI6" s="238"/>
+      <c r="EJ6" s="238"/>
+      <c r="EK6" s="238"/>
+      <c r="EL6" s="238"/>
+      <c r="EM6" s="238"/>
+      <c r="EN6" s="238"/>
+      <c r="EO6" s="238"/>
+      <c r="EP6" s="238"/>
+      <c r="EQ6" s="238"/>
+      <c r="ER6" s="238"/>
+      <c r="ES6" s="238"/>
+      <c r="ET6" s="238"/>
+      <c r="EU6" s="238"/>
+      <c r="EV6" s="239"/>
+      <c r="EW6" s="242">
         <v>6</v>
       </c>
-      <c r="EX6" s="242"/>
-      <c r="EY6" s="242"/>
-      <c r="EZ6" s="242"/>
-      <c r="FA6" s="242"/>
-      <c r="FB6" s="242"/>
-      <c r="FC6" s="242"/>
-      <c r="FD6" s="242"/>
-      <c r="FE6" s="242"/>
-      <c r="FF6" s="242"/>
-      <c r="FG6" s="242"/>
-      <c r="FH6" s="242"/>
-      <c r="FI6" s="242"/>
-      <c r="FJ6" s="242"/>
-      <c r="FK6" s="242"/>
-      <c r="FL6" s="242"/>
-      <c r="FM6" s="242"/>
-      <c r="FN6" s="242"/>
-      <c r="FO6" s="242"/>
-      <c r="FP6" s="242"/>
-      <c r="FQ6" s="242"/>
-      <c r="FR6" s="242"/>
-      <c r="FS6" s="242"/>
-      <c r="FT6" s="242"/>
-      <c r="FU6" s="242"/>
-      <c r="FV6" s="242"/>
-      <c r="FW6" s="242"/>
-      <c r="FX6" s="242"/>
-      <c r="FY6" s="242"/>
-      <c r="FZ6" s="243"/>
-      <c r="GA6" s="237">
+      <c r="EX6" s="243"/>
+      <c r="EY6" s="243"/>
+      <c r="EZ6" s="243"/>
+      <c r="FA6" s="243"/>
+      <c r="FB6" s="243"/>
+      <c r="FC6" s="243"/>
+      <c r="FD6" s="243"/>
+      <c r="FE6" s="243"/>
+      <c r="FF6" s="243"/>
+      <c r="FG6" s="243"/>
+      <c r="FH6" s="243"/>
+      <c r="FI6" s="243"/>
+      <c r="FJ6" s="243"/>
+      <c r="FK6" s="243"/>
+      <c r="FL6" s="243"/>
+      <c r="FM6" s="243"/>
+      <c r="FN6" s="243"/>
+      <c r="FO6" s="243"/>
+      <c r="FP6" s="243"/>
+      <c r="FQ6" s="243"/>
+      <c r="FR6" s="243"/>
+      <c r="FS6" s="243"/>
+      <c r="FT6" s="243"/>
+      <c r="FU6" s="243"/>
+      <c r="FV6" s="243"/>
+      <c r="FW6" s="243"/>
+      <c r="FX6" s="243"/>
+      <c r="FY6" s="243"/>
+      <c r="FZ6" s="244"/>
+      <c r="GA6" s="238">
         <v>7</v>
       </c>
-      <c r="GB6" s="237"/>
-      <c r="GC6" s="237"/>
-      <c r="GD6" s="237"/>
-      <c r="GE6" s="237"/>
-      <c r="GF6" s="237"/>
-      <c r="GG6" s="237"/>
-      <c r="GH6" s="237"/>
-      <c r="GI6" s="237"/>
-      <c r="GJ6" s="237"/>
-      <c r="GK6" s="237"/>
-      <c r="GL6" s="237"/>
-      <c r="GM6" s="237"/>
-      <c r="GN6" s="237"/>
-      <c r="GO6" s="237"/>
-      <c r="GP6" s="237"/>
-      <c r="GQ6" s="237"/>
-      <c r="GR6" s="237"/>
-      <c r="GS6" s="237"/>
-      <c r="GT6" s="237"/>
-      <c r="GU6" s="237"/>
-      <c r="GV6" s="237"/>
-      <c r="GW6" s="237"/>
-      <c r="GX6" s="237"/>
-      <c r="GY6" s="237"/>
-      <c r="GZ6" s="237"/>
-      <c r="HA6" s="237"/>
-      <c r="HB6" s="237"/>
-      <c r="HC6" s="237"/>
-      <c r="HD6" s="237"/>
-      <c r="HE6" s="238"/>
-      <c r="HF6" s="237">
+      <c r="GB6" s="238"/>
+      <c r="GC6" s="238"/>
+      <c r="GD6" s="238"/>
+      <c r="GE6" s="238"/>
+      <c r="GF6" s="238"/>
+      <c r="GG6" s="238"/>
+      <c r="GH6" s="238"/>
+      <c r="GI6" s="238"/>
+      <c r="GJ6" s="238"/>
+      <c r="GK6" s="238"/>
+      <c r="GL6" s="238"/>
+      <c r="GM6" s="238"/>
+      <c r="GN6" s="238"/>
+      <c r="GO6" s="238"/>
+      <c r="GP6" s="238"/>
+      <c r="GQ6" s="238"/>
+      <c r="GR6" s="238"/>
+      <c r="GS6" s="238"/>
+      <c r="GT6" s="238"/>
+      <c r="GU6" s="238"/>
+      <c r="GV6" s="238"/>
+      <c r="GW6" s="238"/>
+      <c r="GX6" s="238"/>
+      <c r="GY6" s="238"/>
+      <c r="GZ6" s="238"/>
+      <c r="HA6" s="238"/>
+      <c r="HB6" s="238"/>
+      <c r="HC6" s="238"/>
+      <c r="HD6" s="238"/>
+      <c r="HE6" s="239"/>
+      <c r="HF6" s="238">
         <v>8</v>
       </c>
-      <c r="HG6" s="237"/>
-      <c r="HH6" s="237"/>
-      <c r="HI6" s="237"/>
-      <c r="HJ6" s="237"/>
-      <c r="HK6" s="237"/>
-      <c r="HL6" s="237"/>
-      <c r="HM6" s="237"/>
-      <c r="HN6" s="237"/>
-      <c r="HO6" s="237"/>
-      <c r="HP6" s="237"/>
-      <c r="HQ6" s="237"/>
-      <c r="HR6" s="237"/>
-      <c r="HS6" s="237"/>
-      <c r="HT6" s="237"/>
-      <c r="HU6" s="237"/>
-      <c r="HV6" s="237"/>
-      <c r="HW6" s="237"/>
-      <c r="HX6" s="237"/>
-      <c r="HY6" s="237"/>
-      <c r="HZ6" s="237"/>
-      <c r="IA6" s="237"/>
-      <c r="IB6" s="237"/>
-      <c r="IC6" s="237"/>
-      <c r="ID6" s="237"/>
-      <c r="IE6" s="237"/>
-      <c r="IF6" s="237"/>
-      <c r="IG6" s="237"/>
-      <c r="IH6" s="237"/>
-      <c r="II6" s="237"/>
-      <c r="IJ6" s="238"/>
-      <c r="IK6" s="241">
+      <c r="HG6" s="238"/>
+      <c r="HH6" s="238"/>
+      <c r="HI6" s="238"/>
+      <c r="HJ6" s="238"/>
+      <c r="HK6" s="238"/>
+      <c r="HL6" s="238"/>
+      <c r="HM6" s="238"/>
+      <c r="HN6" s="238"/>
+      <c r="HO6" s="238"/>
+      <c r="HP6" s="238"/>
+      <c r="HQ6" s="238"/>
+      <c r="HR6" s="238"/>
+      <c r="HS6" s="238"/>
+      <c r="HT6" s="238"/>
+      <c r="HU6" s="238"/>
+      <c r="HV6" s="238"/>
+      <c r="HW6" s="238"/>
+      <c r="HX6" s="238"/>
+      <c r="HY6" s="238"/>
+      <c r="HZ6" s="238"/>
+      <c r="IA6" s="238"/>
+      <c r="IB6" s="238"/>
+      <c r="IC6" s="238"/>
+      <c r="ID6" s="238"/>
+      <c r="IE6" s="238"/>
+      <c r="IF6" s="238"/>
+      <c r="IG6" s="238"/>
+      <c r="IH6" s="238"/>
+      <c r="II6" s="238"/>
+      <c r="IJ6" s="239"/>
+      <c r="IK6" s="242">
         <v>9</v>
       </c>
-      <c r="IL6" s="242"/>
-      <c r="IM6" s="242"/>
-      <c r="IN6" s="242"/>
-      <c r="IO6" s="242"/>
-      <c r="IP6" s="242"/>
-      <c r="IQ6" s="242"/>
-      <c r="IR6" s="242"/>
-      <c r="IS6" s="242"/>
-      <c r="IT6" s="242"/>
-      <c r="IU6" s="242"/>
-      <c r="IV6" s="242"/>
-      <c r="IW6" s="242"/>
-      <c r="IX6" s="242"/>
-      <c r="IY6" s="242"/>
-      <c r="IZ6" s="242"/>
-      <c r="JA6" s="242"/>
-      <c r="JB6" s="242"/>
-      <c r="JC6" s="242"/>
-      <c r="JD6" s="242"/>
-      <c r="JE6" s="242"/>
-      <c r="JF6" s="242"/>
-      <c r="JG6" s="242"/>
-      <c r="JH6" s="242"/>
-      <c r="JI6" s="242"/>
-      <c r="JJ6" s="242"/>
-      <c r="JK6" s="242"/>
-      <c r="JL6" s="242"/>
-      <c r="JM6" s="242"/>
-      <c r="JN6" s="243"/>
-      <c r="JO6" s="237">
+      <c r="IL6" s="243"/>
+      <c r="IM6" s="243"/>
+      <c r="IN6" s="243"/>
+      <c r="IO6" s="243"/>
+      <c r="IP6" s="243"/>
+      <c r="IQ6" s="243"/>
+      <c r="IR6" s="243"/>
+      <c r="IS6" s="243"/>
+      <c r="IT6" s="243"/>
+      <c r="IU6" s="243"/>
+      <c r="IV6" s="243"/>
+      <c r="IW6" s="243"/>
+      <c r="IX6" s="243"/>
+      <c r="IY6" s="243"/>
+      <c r="IZ6" s="243"/>
+      <c r="JA6" s="243"/>
+      <c r="JB6" s="243"/>
+      <c r="JC6" s="243"/>
+      <c r="JD6" s="243"/>
+      <c r="JE6" s="243"/>
+      <c r="JF6" s="243"/>
+      <c r="JG6" s="243"/>
+      <c r="JH6" s="243"/>
+      <c r="JI6" s="243"/>
+      <c r="JJ6" s="243"/>
+      <c r="JK6" s="243"/>
+      <c r="JL6" s="243"/>
+      <c r="JM6" s="243"/>
+      <c r="JN6" s="244"/>
+      <c r="JO6" s="238">
         <v>10</v>
       </c>
-      <c r="JP6" s="237"/>
-      <c r="JQ6" s="237"/>
-      <c r="JR6" s="237"/>
-      <c r="JS6" s="237"/>
-      <c r="JT6" s="237"/>
-      <c r="JU6" s="237"/>
-      <c r="JV6" s="237"/>
-      <c r="JW6" s="237"/>
-      <c r="JX6" s="237"/>
-      <c r="JY6" s="237"/>
-      <c r="JZ6" s="237"/>
-      <c r="KA6" s="237"/>
-      <c r="KB6" s="237"/>
-      <c r="KC6" s="237"/>
-      <c r="KD6" s="237"/>
-      <c r="KE6" s="237"/>
-      <c r="KF6" s="237"/>
-      <c r="KG6" s="237"/>
-      <c r="KH6" s="237"/>
-      <c r="KI6" s="237"/>
-      <c r="KJ6" s="237"/>
-      <c r="KK6" s="237"/>
-      <c r="KL6" s="237"/>
-      <c r="KM6" s="237"/>
-      <c r="KN6" s="237"/>
-      <c r="KO6" s="237"/>
-      <c r="KP6" s="237"/>
-      <c r="KQ6" s="237"/>
-      <c r="KR6" s="237"/>
-      <c r="KS6" s="238"/>
-      <c r="KT6" s="241">
+      <c r="JP6" s="238"/>
+      <c r="JQ6" s="238"/>
+      <c r="JR6" s="238"/>
+      <c r="JS6" s="238"/>
+      <c r="JT6" s="238"/>
+      <c r="JU6" s="238"/>
+      <c r="JV6" s="238"/>
+      <c r="JW6" s="238"/>
+      <c r="JX6" s="238"/>
+      <c r="JY6" s="238"/>
+      <c r="JZ6" s="238"/>
+      <c r="KA6" s="238"/>
+      <c r="KB6" s="238"/>
+      <c r="KC6" s="238"/>
+      <c r="KD6" s="238"/>
+      <c r="KE6" s="238"/>
+      <c r="KF6" s="238"/>
+      <c r="KG6" s="238"/>
+      <c r="KH6" s="238"/>
+      <c r="KI6" s="238"/>
+      <c r="KJ6" s="238"/>
+      <c r="KK6" s="238"/>
+      <c r="KL6" s="238"/>
+      <c r="KM6" s="238"/>
+      <c r="KN6" s="238"/>
+      <c r="KO6" s="238"/>
+      <c r="KP6" s="238"/>
+      <c r="KQ6" s="238"/>
+      <c r="KR6" s="238"/>
+      <c r="KS6" s="239"/>
+      <c r="KT6" s="242">
         <v>11</v>
       </c>
-      <c r="KU6" s="242"/>
-      <c r="KV6" s="242"/>
-      <c r="KW6" s="242"/>
-      <c r="KX6" s="242"/>
-      <c r="KY6" s="242"/>
-      <c r="KZ6" s="242"/>
-      <c r="LA6" s="242"/>
-      <c r="LB6" s="242"/>
-      <c r="LC6" s="242"/>
-      <c r="LD6" s="242"/>
-      <c r="LE6" s="242"/>
-      <c r="LF6" s="242"/>
-      <c r="LG6" s="242"/>
-      <c r="LH6" s="242"/>
-      <c r="LI6" s="242"/>
-      <c r="LJ6" s="242"/>
-      <c r="LK6" s="242"/>
-      <c r="LL6" s="242"/>
-      <c r="LM6" s="242"/>
-      <c r="LN6" s="242"/>
-      <c r="LO6" s="242"/>
-      <c r="LP6" s="242"/>
-      <c r="LQ6" s="242"/>
-      <c r="LR6" s="242"/>
-      <c r="LS6" s="242"/>
-      <c r="LT6" s="242"/>
-      <c r="LU6" s="242"/>
-      <c r="LV6" s="242"/>
-      <c r="LW6" s="243"/>
-      <c r="LX6" s="237">
+      <c r="KU6" s="243"/>
+      <c r="KV6" s="243"/>
+      <c r="KW6" s="243"/>
+      <c r="KX6" s="243"/>
+      <c r="KY6" s="243"/>
+      <c r="KZ6" s="243"/>
+      <c r="LA6" s="243"/>
+      <c r="LB6" s="243"/>
+      <c r="LC6" s="243"/>
+      <c r="LD6" s="243"/>
+      <c r="LE6" s="243"/>
+      <c r="LF6" s="243"/>
+      <c r="LG6" s="243"/>
+      <c r="LH6" s="243"/>
+      <c r="LI6" s="243"/>
+      <c r="LJ6" s="243"/>
+      <c r="LK6" s="243"/>
+      <c r="LL6" s="243"/>
+      <c r="LM6" s="243"/>
+      <c r="LN6" s="243"/>
+      <c r="LO6" s="243"/>
+      <c r="LP6" s="243"/>
+      <c r="LQ6" s="243"/>
+      <c r="LR6" s="243"/>
+      <c r="LS6" s="243"/>
+      <c r="LT6" s="243"/>
+      <c r="LU6" s="243"/>
+      <c r="LV6" s="243"/>
+      <c r="LW6" s="244"/>
+      <c r="LX6" s="238">
         <v>12</v>
       </c>
-      <c r="LY6" s="237"/>
-      <c r="LZ6" s="237"/>
-      <c r="MA6" s="237"/>
-      <c r="MB6" s="237"/>
-      <c r="MC6" s="237"/>
-      <c r="MD6" s="237"/>
-      <c r="ME6" s="237"/>
-      <c r="MF6" s="237"/>
-      <c r="MG6" s="237"/>
-      <c r="MH6" s="237"/>
-      <c r="MI6" s="237"/>
-      <c r="MJ6" s="237"/>
-      <c r="MK6" s="237"/>
-      <c r="ML6" s="237"/>
-      <c r="MM6" s="237"/>
-      <c r="MN6" s="237"/>
-      <c r="MO6" s="237"/>
-      <c r="MP6" s="237"/>
-      <c r="MQ6" s="237"/>
-      <c r="MR6" s="237"/>
-      <c r="MS6" s="237"/>
-      <c r="MT6" s="237"/>
-      <c r="MU6" s="237"/>
-      <c r="MV6" s="237"/>
-      <c r="MW6" s="237"/>
-      <c r="MX6" s="237"/>
-      <c r="MY6" s="237"/>
-      <c r="MZ6" s="237"/>
-      <c r="NA6" s="237"/>
-      <c r="NB6" s="238"/>
+      <c r="LY6" s="238"/>
+      <c r="LZ6" s="238"/>
+      <c r="MA6" s="238"/>
+      <c r="MB6" s="238"/>
+      <c r="MC6" s="238"/>
+      <c r="MD6" s="238"/>
+      <c r="ME6" s="238"/>
+      <c r="MF6" s="238"/>
+      <c r="MG6" s="238"/>
+      <c r="MH6" s="238"/>
+      <c r="MI6" s="238"/>
+      <c r="MJ6" s="238"/>
+      <c r="MK6" s="238"/>
+      <c r="ML6" s="238"/>
+      <c r="MM6" s="238"/>
+      <c r="MN6" s="238"/>
+      <c r="MO6" s="238"/>
+      <c r="MP6" s="238"/>
+      <c r="MQ6" s="238"/>
+      <c r="MR6" s="238"/>
+      <c r="MS6" s="238"/>
+      <c r="MT6" s="238"/>
+      <c r="MU6" s="238"/>
+      <c r="MV6" s="238"/>
+      <c r="MW6" s="238"/>
+      <c r="MX6" s="238"/>
+      <c r="MY6" s="238"/>
+      <c r="MZ6" s="238"/>
+      <c r="NA6" s="238"/>
+      <c r="NB6" s="239"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -37358,7 +37362,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="244" t="s">
+      <c r="A8" s="245" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -37750,7 +37754,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="244"/>
+      <c r="A9" s="245"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -38132,7 +38136,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="244"/>
+      <c r="A10" s="245"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -38514,7 +38518,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="244"/>
+      <c r="A11" s="245"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -38890,7 +38894,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="244"/>
+      <c r="A12" s="245"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -39264,7 +39268,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="244"/>
+      <c r="A13" s="245"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -39634,7 +39638,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="244"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -40004,7 +40008,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="245" t="s">
+      <c r="A15" s="246" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="75"/>
@@ -40384,7 +40388,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="244"/>
+      <c r="A16" s="245"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -40756,7 +40760,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="244"/>
+      <c r="A17" s="245"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -41124,7 +41128,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="244"/>
+      <c r="A18" s="245"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -41494,7 +41498,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="244"/>
+      <c r="A19" s="245"/>
       <c r="B19" s="85"/>
       <c r="C19" s="71"/>
       <c r="D19" s="71"/>
@@ -41862,7 +41866,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="244" t="s">
+      <c r="A20" s="245" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="42"/>
@@ -42246,7 +42250,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="244"/>
+      <c r="A21" s="245"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -42623,7 +42627,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="244"/>
+      <c r="A22" s="245"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -43003,7 +43007,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="244"/>
+      <c r="A23" s="245"/>
       <c r="B23" s="24"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -43379,7 +43383,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="244"/>
+      <c r="A24" s="245"/>
       <c r="B24" s="26"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -43749,7 +43753,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="244" t="s">
+      <c r="A25" s="245" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="75"/>
@@ -44129,7 +44133,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="244"/>
+      <c r="A26" s="245"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -44505,7 +44509,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="244"/>
+      <c r="A27" s="245"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -44877,7 +44881,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="244"/>
+      <c r="A28" s="245"/>
       <c r="B28" s="24"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -45250,7 +45254,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="244"/>
+      <c r="A29" s="245"/>
       <c r="B29" s="91"/>
       <c r="C29" s="92"/>
       <c r="D29" s="92"/>
@@ -45620,7 +45624,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="245" t="s">
+      <c r="A30" s="246" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -45992,7 +45996,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="244"/>
+      <c r="A31" s="245"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -46366,7 +46370,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="244"/>
+      <c r="A32" s="245"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -46740,7 +46744,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="244"/>
+      <c r="A33" s="245"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -47110,7 +47114,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="244"/>
+      <c r="A34" s="245"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -47478,7 +47482,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="244" t="s">
+      <c r="A35" s="245" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -47860,7 +47864,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="244"/>
+      <c r="A36" s="245"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -48232,7 +48236,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="244"/>
+      <c r="A37" s="245"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -48608,7 +48612,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="244"/>
+      <c r="A38" s="245"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -48982,7 +48986,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="244"/>
+      <c r="A39" s="245"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -49354,7 +49358,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="244" t="s">
+      <c r="A40" s="245" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -49732,7 +49736,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="244"/>
+      <c r="A41" s="245"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -50108,7 +50112,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="244"/>
+      <c r="A42" s="245"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -50478,7 +50482,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="244"/>
+      <c r="A43" s="245"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -50848,7 +50852,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="244"/>
+      <c r="A44" s="245"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -51216,7 +51220,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="244" t="s">
+      <c r="A45" s="245" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -51596,7 +51600,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="244"/>
+      <c r="A46" s="245"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -51966,7 +51970,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="244"/>
+      <c r="A47" s="245"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -52342,7 +52346,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="244"/>
+      <c r="A48" s="245"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -52712,7 +52716,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="244"/>
+      <c r="A49" s="245"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -53086,7 +53090,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="244" t="s">
+      <c r="A50" s="245" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -53468,7 +53472,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="244"/>
+      <c r="A51" s="245"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -53846,7 +53850,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="244"/>
+      <c r="A52" s="245"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -54218,7 +54222,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="244"/>
+      <c r="A53" s="245"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -54588,7 +54592,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="244"/>
+      <c r="A54" s="245"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -54976,15 +54980,6 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="A35:A39"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="B6:AF6"/>
     <mergeCell ref="AG6:BH6"/>
@@ -54997,6 +54992,15 @@
     <mergeCell ref="IK6:JN6"/>
     <mergeCell ref="JO6:KS6"/>
     <mergeCell ref="KT6:LW6"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A35:A39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -55010,8 +55014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -55029,43 +55033,43 @@
   <sheetData>
     <row r="1" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="257" t="s">
+      <c r="B2" s="258" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="254" t="s">
+      <c r="C2" s="255" t="s">
         <v>161</v>
       </c>
-      <c r="D2" s="255"/>
-      <c r="E2" s="255"/>
-      <c r="F2" s="256"/>
-      <c r="G2" s="249" t="s">
+      <c r="D2" s="256"/>
+      <c r="E2" s="256"/>
+      <c r="F2" s="257"/>
+      <c r="G2" s="250" t="s">
         <v>126</v>
       </c>
-      <c r="H2" s="250"/>
-      <c r="I2" s="250"/>
-      <c r="J2" s="251"/>
+      <c r="H2" s="251"/>
+      <c r="I2" s="251"/>
+      <c r="J2" s="252"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="258"/>
-      <c r="C3" s="261" t="s">
+      <c r="B3" s="259"/>
+      <c r="C3" s="262" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="252"/>
-      <c r="E3" s="252" t="s">
+      <c r="D3" s="253"/>
+      <c r="E3" s="253" t="s">
         <v>159</v>
       </c>
-      <c r="F3" s="253"/>
-      <c r="G3" s="262" t="s">
+      <c r="F3" s="254"/>
+      <c r="G3" s="263" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="247"/>
-      <c r="I3" s="247" t="s">
+      <c r="H3" s="248"/>
+      <c r="I3" s="248" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="248"/>
+      <c r="J3" s="249"/>
     </row>
     <row r="4" spans="2:10" s="167" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="258"/>
+      <c r="B4" s="259"/>
       <c r="C4" s="185" t="s">
         <v>122</v>
       </c>
@@ -55100,7 +55104,7 @@
       <c r="D5" s="183"/>
       <c r="E5" s="183">
         <f>SUM(E6:E38)</f>
-        <v>6.5</v>
+        <v>12.5</v>
       </c>
       <c r="F5" s="184"/>
       <c r="G5" s="194">
@@ -55136,7 +55140,7 @@
       <c r="J6" s="177"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="246">
+      <c r="B7" s="247">
         <v>43219</v>
       </c>
       <c r="C7" s="197">
@@ -55157,7 +55161,7 @@
       <c r="J7" s="203"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="246"/>
+      <c r="B8" s="247"/>
       <c r="C8" s="204"/>
       <c r="D8" s="205"/>
       <c r="E8" s="206"/>
@@ -55189,7 +55193,7 @@
       <c r="J9" s="177"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="246">
+      <c r="B10" s="247">
         <v>43221</v>
       </c>
       <c r="C10" s="211">
@@ -55210,7 +55214,7 @@
       <c r="J10" s="200"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="246"/>
+      <c r="B11" s="247"/>
       <c r="C11" s="213">
         <v>2</v>
       </c>
@@ -55225,7 +55229,7 @@
       <c r="J11" s="220"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="246"/>
+      <c r="B12" s="247"/>
       <c r="C12" s="213">
         <v>1</v>
       </c>
@@ -55240,7 +55244,7 @@
       <c r="J12" s="220"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="246"/>
+      <c r="B13" s="247"/>
       <c r="C13" s="221">
         <v>1</v>
       </c>
@@ -55255,7 +55259,7 @@
       <c r="J13" s="207"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="259">
+      <c r="B14" s="260">
         <v>43222</v>
       </c>
       <c r="C14" s="197">
@@ -55276,7 +55280,7 @@
       <c r="J14" s="200"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="260"/>
+      <c r="B15" s="261"/>
       <c r="C15" s="204">
         <v>0.5</v>
       </c>
@@ -55316,7 +55320,7 @@
       <c r="J16" s="180"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="259">
+      <c r="B17" s="260">
         <v>43226</v>
       </c>
       <c r="C17" s="197"/>
@@ -55341,7 +55345,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="260"/>
+      <c r="B18" s="261"/>
       <c r="C18" s="204"/>
       <c r="D18" s="205"/>
       <c r="E18" s="206"/>
@@ -55449,7 +55453,7 @@
       <c r="J23" s="177"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="246">
+      <c r="B24" s="247">
         <v>43235</v>
       </c>
       <c r="C24" s="197">
@@ -55470,7 +55474,7 @@
       <c r="J24" s="200"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="246"/>
+      <c r="B25" s="247"/>
       <c r="C25" s="204">
         <v>2</v>
       </c>
@@ -55489,7 +55493,7 @@
       <c r="J25" s="210"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="246">
+      <c r="B26" s="247">
         <v>43236</v>
       </c>
       <c r="C26" s="197">
@@ -55510,7 +55514,7 @@
       <c r="J26" s="200"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="246"/>
+      <c r="B27" s="247"/>
       <c r="C27" s="223">
         <v>0.5</v>
       </c>
@@ -55529,7 +55533,7 @@
       <c r="J27" s="226"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="246"/>
+      <c r="B28" s="247"/>
       <c r="C28" s="223">
         <v>3</v>
       </c>
@@ -55544,7 +55548,7 @@
       <c r="J28" s="226"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="246"/>
+      <c r="B29" s="247"/>
       <c r="C29" s="223">
         <v>2</v>
       </c>
@@ -55559,7 +55563,7 @@
       <c r="J29" s="226"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="246"/>
+      <c r="B30" s="247"/>
       <c r="C30" s="204">
         <v>1</v>
       </c>
@@ -55594,7 +55598,7 @@
       <c r="B32" s="179">
         <v>43242</v>
       </c>
-      <c r="C32" s="264"/>
+      <c r="C32" s="233"/>
       <c r="D32" s="188"/>
       <c r="E32" s="186">
         <v>3</v>
@@ -55612,11 +55616,17 @@
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="179"/>
+      <c r="B33" s="179">
+        <v>43243</v>
+      </c>
       <c r="C33" s="176"/>
       <c r="D33" s="188"/>
-      <c r="E33" s="186"/>
-      <c r="F33" s="177"/>
+      <c r="E33" s="186">
+        <v>6</v>
+      </c>
+      <c r="F33" s="177" t="s">
+        <v>184</v>
+      </c>
       <c r="G33" s="178"/>
       <c r="H33" s="188"/>
       <c r="I33" s="186"/>
@@ -55744,7 +55754,7 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="263">
+      <c r="B4" s="264">
         <v>43237</v>
       </c>
       <c r="C4" s="190" t="s">
@@ -55753,35 +55763,35 @@
       <c r="D4" s="190"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="263"/>
+      <c r="B5" s="264"/>
       <c r="C5" s="190" t="s">
         <v>172</v>
       </c>
       <c r="D5" s="190"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="263"/>
+      <c r="B6" s="264"/>
       <c r="C6" s="190" t="s">
         <v>173</v>
       </c>
       <c r="D6" s="190"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="263"/>
+      <c r="B7" s="264"/>
       <c r="C7" s="190" t="s">
         <v>174</v>
       </c>
       <c r="D7" s="190"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="263"/>
+      <c r="B8" s="264"/>
       <c r="C8" s="190" t="s">
         <v>175</v>
       </c>
       <c r="D8" s="190"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="263"/>
+      <c r="B9" s="264"/>
       <c r="C9" s="190" t="s">
         <v>176</v>
       </c>
@@ -55790,7 +55800,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="263"/>
+      <c r="B10" s="264"/>
       <c r="C10" s="232" t="s">
         <v>180</v>
       </c>
@@ -55799,7 +55809,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="263"/>
+      <c r="B11" s="264"/>
       <c r="C11" s="190" t="s">
         <v>178</v>
       </c>

</xml_diff>